<commit_message>
move shielding to hdmi, trace cleanup
</commit_message>
<xml_diff>
--- a/nubus-to-ztex/signals.xlsx
+++ b/nubus-to-ztex/signals.xlsx
@@ -949,115 +949,115 @@
     <t xml:space="preserve">T4</t>
   </si>
   <si>
+    <t xml:space="preserve">SD_D2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T6~IO_L23N_T3_34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tm_n_o0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U4~IO_L8P_T1_34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SD_D3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R6~IO_L19P_T3_34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tm_oe_n2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U3~IO_L8N_T1_34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SD_CMD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R5~IO_L19N_T3_VREF_34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VREF Bank 34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tm_o_n2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V1~IO_L7N_T1_34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SD_CLK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V2~IO_L9N_T1_DQS_34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tm_n1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U1~IO_L7P_T1_34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SD_D0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U2~IO_L9P_T1_DQS_34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tm_n0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T3~IO_L11N_T1_SRCC_34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T3</t>
+  </si>
+  <si>
     <t xml:space="preserve">SD_D1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T6~IO_L23N_T3_34</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tm_n_o0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U4~IO_L8P_T1_34</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SD_D0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R6~IO_L19P_T3_34</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tm_oe_n2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U3~IO_L8N_T1_34</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SD_CLK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R5~IO_L19N_T3_VREF_34</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VREF Bank 34</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tm_o_n2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">V1~IO_L7N_T1_34</t>
-  </si>
-  <si>
-    <t xml:space="preserve">V1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SD_CMD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">V2~IO_L9N_T1_DQS_34</t>
-  </si>
-  <si>
-    <t xml:space="preserve">V2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tm_n0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U1~IO_L7P_T1_34</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SD_D3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U2~IO_L9P_T1_DQS_34</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tm_n1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T3~IO_L11N_T1_SRCC_34</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SD_D2</t>
   </si>
   <si>
     <t xml:space="preserve">K6~IO_0_34</t>
@@ -2923,16 +2923,6 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -3003,8 +2993,8 @@
   </sheetPr>
   <dimension ref="A1:AG232"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="S93" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AC99" activeCellId="0" sqref="AC99"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F61" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J89" activeCellId="0" sqref="J89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3343,8 +3333,7 @@
       <c r="U9" s="30" t="str">
         <f aca="false">IF(AND(K9&lt;&gt;"",K9&lt;&gt;"+3v3",K9&lt;&gt;"GND"),CONCATENATE("set_property PACKAGE_PIN ",D9," [get_ports {",K9,"}]",CHAR(10),"set_property IOSTANDARD LVTTL [get_ports {",K9,"}]",CHAR(10)),"")</f>
         <v>set_property PACKAGE_PIN K16 [get_ports {nmrq_n}]
-set_property IOSTANDARD LVTTL [get_ports {nmrq_n}]
-</v>
+set_property IOSTANDARD LVTTL [get_ports {nmrq_n}]</v>
       </c>
       <c r="V9" s="31" t="str">
         <f aca="false">IF(AND(K9&lt;&gt;"",K9&lt;&gt;"+3v3",K9&lt;&gt;"GND",NOT(ISNA(P9)),NOT(ISNA(N9))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S9/$V$8,"0.000")," [get_ports {",K9,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S9/$W$8,"0.000")," [get_ports {",K9,"}]",CHAR(10)),"")</f>
@@ -3418,26 +3407,22 @@
       <c r="U10" s="30" t="str">
         <f aca="false">IF(AND(K10&lt;&gt;"",K10&lt;&gt;"+3v3",K10&lt;&gt;"GND"),CONCATENATE("set_property PACKAGE_PIN ",D10," [get_ports {",K10,"}]",CHAR(10),"set_property IOSTANDARD LVTTL [get_ports {",K10,"}]",CHAR(10)),"")</f>
         <v>set_property PACKAGE_PIN J18 [get_ports {rqst_n}]
-set_property IOSTANDARD LVTTL [get_ports {rqst_n}]
-</v>
+set_property IOSTANDARD LVTTL [get_ports {rqst_n}]</v>
       </c>
       <c r="V10" s="31" t="str">
         <f aca="false">IF(AND(K10&lt;&gt;"",K10&lt;&gt;"+3v3",K10&lt;&gt;"GND",NOT(ISNA(P10)),NOT(ISNA(N10))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S10/$V$8,"0.000")," [get_ports {",K10,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S10/$W$8,"0.000")," [get_ports {",K10,"}]",CHAR(10)),"")</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.404 [get_ports {rqst_n}]
-set_input_delay -clock clk_3v3_n -max 52.456 [get_ports {rqst_n}]
-</v>
+set_input_delay -clock clk_3v3_n -max 52.456 [get_ports {rqst_n}]</v>
       </c>
       <c r="W10" s="31" t="str">
         <f aca="false">IF(AND(K10&lt;&gt;"",K10&lt;&gt;"+3v3",K10&lt;&gt;"GND",NOT(ISNA(P10)),NOT(ISNA(N10))),CONCATENATE("set_output_delay -clock clk_3v3_n -min ",TEXT(-$W$6+P10/$V$8+$P$136/$V$8,"0.000")," [get_ports {",K10,"}]",CHAR(10),"set_output_delay -clock clk_3v3_n -max ",TEXT(0.25+0.25+$W$5+P10/$W$8+$P$136/$W$8,"0.000")," [get_ports {",K10,"}]",CHAR(10)),"")</f>
         <v>set_output_delay -clock clk_3v3_n -min -6.155 [get_ports {rqst_n}]
-set_output_delay -clock clk_3v3_n -max 53.627 [get_ports {rqst_n}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.627 [get_ports {rqst_n}]</v>
       </c>
       <c r="Y10" s="7" t="str">
         <f aca="false">CONCATENATE(IF(OR(T10="IO",T10="I"),V10,""),IF(OR(T10="IO",T10="O"),W10,""))</f>
         <v>set_output_delay -clock clk_3v3_n -min -6.155 [get_ports {rqst_n}]
-set_output_delay -clock clk_3v3_n -max 53.627 [get_ports {rqst_n}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.627 [get_ports {rqst_n}]</v>
       </c>
       <c r="AG10" s="8" t="str">
         <f aca="false">IF(OR(LEFT(K10,3)="LED",LEFT(K10,16)="SBUS_DATA_OE_LED"),CONCATENATE("(",CHAR(34),"user_led",CHAR(34),", 0, Pins(",CHAR(34),D10,CHAR(34),"),  IOStandard(",CHAR(34),"lvcmos33",CHAR(34),")), ",CHAR(35),K10),"")</f>
@@ -3499,28 +3484,24 @@
       <c r="U11" s="30" t="str">
         <f aca="false">IF(AND(K11&lt;&gt;"",K11&lt;&gt;"+3v3",K11&lt;&gt;"GND"),CONCATENATE("set_property PACKAGE_PIN ",D11," [get_ports {",K11,"}]",CHAR(10),"set_property IOSTANDARD LVTTL [get_ports {",K11,"}]",CHAR(10)),"")</f>
         <v>set_property PACKAGE_PIN K15 [get_ports {start_n}]
-set_property IOSTANDARD LVTTL [get_ports {start_n}]
-</v>
+set_property IOSTANDARD LVTTL [get_ports {start_n}]</v>
       </c>
       <c r="V11" s="31" t="str">
         <f aca="false">IF(AND(K11&lt;&gt;"",K11&lt;&gt;"+3v3",K11&lt;&gt;"GND",NOT(ISNA(P11)),NOT(ISNA(N11))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S11/$V$8,"0.000")," [get_ports {",K11,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S11/$W$8,"0.000")," [get_ports {",K11,"}]",CHAR(10)),"")</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.457 [get_ports {start_n}]
-set_input_delay -clock clk_3v3_n -max 52.526 [get_ports {start_n}]
-</v>
+set_input_delay -clock clk_3v3_n -max 52.526 [get_ports {start_n}]</v>
       </c>
       <c r="W11" s="31" t="str">
         <f aca="false">IF(AND(K11&lt;&gt;"",K11&lt;&gt;"+3v3",K11&lt;&gt;"GND",NOT(ISNA(P11)),NOT(ISNA(N11))),CONCATENATE("set_output_delay -clock clk_3v3_n -min ",TEXT(-$W$6+P11/$V$8+$P$136/$V$8,"0.000")," [get_ports {",K11,"}]",CHAR(10),"set_output_delay -clock clk_3v3_n -max ",TEXT(0.25+0.25+$W$5+P11/$W$8+$P$136/$W$8,"0.000")," [get_ports {",K11,"}]",CHAR(10)),"")</f>
         <v>set_output_delay -clock clk_3v3_n -min -6.102 [get_ports {start_n}]
-set_output_delay -clock clk_3v3_n -max 53.697 [get_ports {start_n}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.697 [get_ports {start_n}]</v>
       </c>
       <c r="Y11" s="32" t="str">
         <f aca="false">CONCATENATE(IF(OR(T11="IO",T11="I"),V11,""),IF(OR(T11="IO",T11="O"),W11,""))</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.457 [get_ports {start_n}]
 set_input_delay -clock clk_3v3_n -max 52.526 [get_ports {start_n}]
 set_output_delay -clock clk_3v3_n -min -6.102 [get_ports {start_n}]
-set_output_delay -clock clk_3v3_n -max 53.697 [get_ports {start_n}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.697 [get_ports {start_n}]</v>
       </c>
       <c r="AG11" s="8" t="str">
         <f aca="false">IF(OR(LEFT(K11,3)="LED",LEFT(K11,16)="SBUS_DATA_OE_LED"),CONCATENATE("(",CHAR(34),"user_led",CHAR(34),", 0, Pins(",CHAR(34),D11,CHAR(34),"),  IOStandard(",CHAR(34),"lvcmos33",CHAR(34),")), ",CHAR(35),K11),"")</f>
@@ -3582,28 +3563,24 @@
       <c r="U12" s="30" t="str">
         <f aca="false">IF(AND(K12&lt;&gt;"",K12&lt;&gt;"+3v3",K12&lt;&gt;"GND"),CONCATENATE("set_property PACKAGE_PIN ",D12," [get_ports {",K12,"}]",CHAR(10),"set_property IOSTANDARD LVTTL [get_ports {",K12,"}]",CHAR(10)),"")</f>
         <v>set_property PACKAGE_PIN J17 [get_ports {ack_n}]
-set_property IOSTANDARD LVTTL [get_ports {ack_n}]
-</v>
+set_property IOSTANDARD LVTTL [get_ports {ack_n}]</v>
       </c>
       <c r="V12" s="31" t="str">
         <f aca="false">IF(AND(K12&lt;&gt;"",K12&lt;&gt;"+3v3",K12&lt;&gt;"GND",NOT(ISNA(P12)),NOT(ISNA(N12))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S12/$V$8,"0.000")," [get_ports {",K12,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S12/$W$8,"0.000")," [get_ports {",K12,"}]",CHAR(10)),"")</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.525 [get_ports {ack_n}]
-set_input_delay -clock clk_3v3_n -max 52.617 [get_ports {ack_n}]
-</v>
+set_input_delay -clock clk_3v3_n -max 52.617 [get_ports {ack_n}]</v>
       </c>
       <c r="W12" s="31" t="str">
         <f aca="false">IF(AND(K12&lt;&gt;"",K12&lt;&gt;"+3v3",K12&lt;&gt;"GND",NOT(ISNA(P12)),NOT(ISNA(N12))),CONCATENATE("set_output_delay -clock clk_3v3_n -min ",TEXT(-$W$6+P12/$V$8+$P$136/$V$8,"0.000")," [get_ports {",K12,"}]",CHAR(10),"set_output_delay -clock clk_3v3_n -max ",TEXT(0.25+0.25+$W$5+P12/$W$8+$P$136/$W$8,"0.000")," [get_ports {",K12,"}]",CHAR(10)),"")</f>
         <v>set_output_delay -clock clk_3v3_n -min -6.034 [get_ports {ack_n}]
-set_output_delay -clock clk_3v3_n -max 53.788 [get_ports {ack_n}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.788 [get_ports {ack_n}]</v>
       </c>
       <c r="Y12" s="32" t="str">
         <f aca="false">CONCATENATE(IF(OR(T12="IO",T12="I"),V12,""),IF(OR(T12="IO",T12="O"),W12,""))</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.525 [get_ports {ack_n}]
 set_input_delay -clock clk_3v3_n -max 52.617 [get_ports {ack_n}]
 set_output_delay -clock clk_3v3_n -min -6.034 [get_ports {ack_n}]
-set_output_delay -clock clk_3v3_n -max 53.788 [get_ports {ack_n}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.788 [get_ports {ack_n}]</v>
       </c>
       <c r="AG12" s="8" t="str">
         <f aca="false">IF(OR(LEFT(K12,3)="LED",LEFT(K12,16)="SBUS_DATA_OE_LED"),CONCATENATE("(",CHAR(34),"user_led",CHAR(34),", 0, Pins(",CHAR(34),D12,CHAR(34),"),  IOStandard(",CHAR(34),"lvcmos33",CHAR(34),")), ",CHAR(35),K12),"")</f>
@@ -3665,8 +3642,7 @@
       <c r="U13" s="30" t="str">
         <f aca="false">IF(AND(K13&lt;&gt;"",K13&lt;&gt;"+3v3",K13&lt;&gt;"GND"),CONCATENATE("set_property PACKAGE_PIN ",D13," [get_ports {",K13,"}]",CHAR(10),"set_property IOSTANDARD LVTTL [get_ports {",K13,"}]",CHAR(10)),"")</f>
         <v>set_property PACKAGE_PIN J15 [get_ports {start_oe_n}]
-set_property IOSTANDARD LVTTL [get_ports {start_oe_n}]
-</v>
+set_property IOSTANDARD LVTTL [get_ports {start_oe_n}]</v>
       </c>
       <c r="V13" s="31" t="str">
         <f aca="false">IF(AND(K13&lt;&gt;"",K13&lt;&gt;"+3v3",K13&lt;&gt;"GND",NOT(ISNA(P13)),NOT(ISNA(N13))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S13/$V$8,"0.000")," [get_ports {",K13,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S13/$W$8,"0.000")," [get_ports {",K13,"}]",CHAR(10)),"")</f>
@@ -3740,8 +3716,7 @@
       <c r="U14" s="30" t="str">
         <f aca="false">IF(AND(K14&lt;&gt;"",K14&lt;&gt;"+3v3",K14&lt;&gt;"GND"),CONCATENATE("set_property PACKAGE_PIN ",D14," [get_ports {",K14,"}]",CHAR(10),"set_property IOSTANDARD LVTTL [get_ports {",K14,"}]",CHAR(10)),"")</f>
         <v>set_property PACKAGE_PIN K13 [get_ports {rqst_o_n}]
-set_property IOSTANDARD LVTTL [get_ports {rqst_o_n}]
-</v>
+set_property IOSTANDARD LVTTL [get_ports {rqst_o_n}]</v>
       </c>
       <c r="V14" s="31" t="str">
         <f aca="false">IF(AND(K14&lt;&gt;"",K14&lt;&gt;"+3v3",K14&lt;&gt;"GND",NOT(ISNA(P14)),NOT(ISNA(N14))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S14/$V$8,"0.000")," [get_ports {",K14,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S14/$W$8,"0.000")," [get_ports {",K14,"}]",CHAR(10)),"")</f>
@@ -3817,8 +3792,7 @@
       <c r="U15" s="30" t="str">
         <f aca="false">IF(AND(K15&lt;&gt;"",K15&lt;&gt;"+3v3",K15&lt;&gt;"GND"),CONCATENATE("set_property PACKAGE_PIN ",D15," [get_ports {",K15,"}]",CHAR(10),"set_property IOSTANDARD LVTTL [get_ports {",K15,"}]",CHAR(10)),"")</f>
         <v>set_property PACKAGE_PIN H15 [get_ports {start_o_n}]
-set_property IOSTANDARD LVTTL [get_ports {start_o_n}]
-</v>
+set_property IOSTANDARD LVTTL [get_ports {start_o_n}]</v>
       </c>
       <c r="V15" s="31" t="str">
         <f aca="false">IF(AND(K15&lt;&gt;"",K15&lt;&gt;"+3v3",K15&lt;&gt;"GND",NOT(ISNA(P15)),NOT(ISNA(N15))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S15/$V$8,"0.000")," [get_ports {",K15,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S15/$W$8,"0.000")," [get_ports {",K15,"}]",CHAR(10)),"")</f>
@@ -3892,8 +3866,7 @@
       <c r="U16" s="30" t="str">
         <f aca="false">IF(AND(K16&lt;&gt;"",K16&lt;&gt;"+3v3",K16&lt;&gt;"GND"),CONCATENATE("set_property PACKAGE_PIN ",D16," [get_ports {",K16,"}]",CHAR(10),"set_property IOSTANDARD LVTTL [get_ports {",K16,"}]",CHAR(10)),"")</f>
         <v>set_property PACKAGE_PIN J13 [get_ports {ack_oe_n}]
-set_property IOSTANDARD LVTTL [get_ports {ack_oe_n}]
-</v>
+set_property IOSTANDARD LVTTL [get_ports {ack_oe_n}]</v>
       </c>
       <c r="V16" s="31" t="str">
         <f aca="false">IF(AND(K16&lt;&gt;"",K16&lt;&gt;"+3v3",K16&lt;&gt;"GND",NOT(ISNA(P16)),NOT(ISNA(N16))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S16/$V$8,"0.000")," [get_ports {",K16,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S16/$W$8,"0.000")," [get_ports {",K16,"}]",CHAR(10)),"")</f>
@@ -3967,8 +3940,7 @@
       <c r="U17" s="30" t="str">
         <f aca="false">IF(AND(K17&lt;&gt;"",K17&lt;&gt;"+3v3",K17&lt;&gt;"GND"),CONCATENATE("set_property PACKAGE_PIN ",D17," [get_ports {",K17,"}]",CHAR(10),"set_property IOSTANDARD LVTTL [get_ports {",K17,"}]",CHAR(10)),"")</f>
         <v>set_property PACKAGE_PIN J14 [get_ports {arb_o_n0}]
-set_property IOSTANDARD LVTTL [get_ports {arb_o_n0}]
-</v>
+set_property IOSTANDARD LVTTL [get_ports {arb_o_n0}]</v>
       </c>
       <c r="V17" s="31" t="str">
         <f aca="false">IF(AND(K17&lt;&gt;"",K17&lt;&gt;"+3v3",K17&lt;&gt;"GND",NOT(ISNA(P17)),NOT(ISNA(N17))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S17/$V$8,"0.000")," [get_ports {",K17,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S17/$W$8,"0.000")," [get_ports {",K17,"}]",CHAR(10)),"")</f>
@@ -4042,8 +4014,7 @@
       <c r="U18" s="30" t="str">
         <f aca="false">IF(AND(K18&lt;&gt;"",K18&lt;&gt;"+3v3",K18&lt;&gt;"GND"),CONCATENATE("set_property PACKAGE_PIN ",D18," [get_ports {",K18,"}]",CHAR(10),"set_property IOSTANDARD LVTTL [get_ports {",K18,"}]",CHAR(10)),"")</f>
         <v>set_property PACKAGE_PIN H14 [get_ports {ack_o_n}]
-set_property IOSTANDARD LVTTL [get_ports {ack_o_n}]
-</v>
+set_property IOSTANDARD LVTTL [get_ports {ack_o_n}]</v>
       </c>
       <c r="V18" s="31" t="str">
         <f aca="false">IF(AND(K18&lt;&gt;"",K18&lt;&gt;"+3v3",K18&lt;&gt;"GND",NOT(ISNA(P18)),NOT(ISNA(N18))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S18/$V$8,"0.000")," [get_ports {",K18,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S18/$W$8,"0.000")," [get_ports {",K18,"}]",CHAR(10)),"")</f>
@@ -4117,8 +4088,7 @@
       <c r="U19" s="30" t="str">
         <f aca="false">IF(AND(K19&lt;&gt;"",K19&lt;&gt;"+3v3",K19&lt;&gt;"GND"),CONCATENATE("set_property PACKAGE_PIN ",D19," [get_ports {",K19,"}]",CHAR(10),"set_property IOSTANDARD LVTTL [get_ports {",K19,"}]",CHAR(10)),"")</f>
         <v>set_property PACKAGE_PIN H17 [get_ports {arb_o_n3}]
-set_property IOSTANDARD LVTTL [get_ports {arb_o_n3}]
-</v>
+set_property IOSTANDARD LVTTL [get_ports {arb_o_n3}]</v>
       </c>
       <c r="V19" s="31" t="str">
         <f aca="false">IF(AND(K19&lt;&gt;"",K19&lt;&gt;"+3v3",K19&lt;&gt;"GND",NOT(ISNA(P19)),NOT(ISNA(N19))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S19/$V$8,"0.000")," [get_ports {",K19,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S19/$W$8,"0.000")," [get_ports {",K19,"}]",CHAR(10)),"")</f>
@@ -4192,8 +4162,7 @@
       <c r="U20" s="30" t="str">
         <f aca="false">IF(AND(K20&lt;&gt;"",K20&lt;&gt;"+3v3",K20&lt;&gt;"GND"),CONCATENATE("set_property PACKAGE_PIN ",D20," [get_ports {",K20,"}]",CHAR(10),"set_property IOSTANDARD LVTTL [get_ports {",K20,"}]",CHAR(10)),"")</f>
         <v>set_property PACKAGE_PIN G14 [get_ports {arb_o_n2}]
-set_property IOSTANDARD LVTTL [get_ports {arb_o_n2}]
-</v>
+set_property IOSTANDARD LVTTL [get_ports {arb_o_n2}]</v>
       </c>
       <c r="V20" s="31" t="str">
         <f aca="false">IF(AND(K20&lt;&gt;"",K20&lt;&gt;"+3v3",K20&lt;&gt;"GND",NOT(ISNA(P20)),NOT(ISNA(N20))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S20/$V$8,"0.000")," [get_ports {",K20,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S20/$W$8,"0.000")," [get_ports {",K20,"}]",CHAR(10)),"")</f>
@@ -4267,8 +4236,7 @@
       <c r="U21" s="30" t="str">
         <f aca="false">IF(AND(K21&lt;&gt;"",K21&lt;&gt;"+3v3",K21&lt;&gt;"GND"),CONCATENATE("set_property PACKAGE_PIN ",D21," [get_ports {",K21,"}]",CHAR(10),"set_property IOSTANDARD LVTTL [get_ports {",K21,"}]",CHAR(10)),"")</f>
         <v>set_property PACKAGE_PIN G17 [get_ports {NUBUS_AD_DIR}]
-set_property IOSTANDARD LVTTL [get_ports {NUBUS_AD_DIR}]
-</v>
+set_property IOSTANDARD LVTTL [get_ports {NUBUS_AD_DIR}]</v>
       </c>
       <c r="V21" s="31" t="str">
         <f aca="false">IF(AND(K21&lt;&gt;"",K21&lt;&gt;"+3v3",K21&lt;&gt;"GND",NOT(ISNA(P21)),NOT(ISNA(N21))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S21/$V$8,"0.000")," [get_ports {",K21,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S21/$W$8,"0.000")," [get_ports {",K21,"}]",CHAR(10)),"")</f>
@@ -4344,8 +4312,7 @@
       <c r="U22" s="30" t="str">
         <f aca="false">IF(AND(K22&lt;&gt;"",K22&lt;&gt;"+3v3",K22&lt;&gt;"GND"),CONCATENATE("set_property PACKAGE_PIN ",D22," [get_ports {",K22,"}]",CHAR(10),"set_property IOSTANDARD LVTTL [get_ports {",K22,"}]",CHAR(10)),"")</f>
         <v>set_property PACKAGE_PIN G16 [get_ports {arb_o_n1}]
-set_property IOSTANDARD LVTTL [get_ports {arb_o_n1}]
-</v>
+set_property IOSTANDARD LVTTL [get_ports {arb_o_n1}]</v>
       </c>
       <c r="V22" s="31" t="str">
         <f aca="false">IF(AND(K22&lt;&gt;"",K22&lt;&gt;"+3v3",K22&lt;&gt;"GND",NOT(ISNA(P22)),NOT(ISNA(N22))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S22/$V$8,"0.000")," [get_ports {",K22,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S22/$W$8,"0.000")," [get_ports {",K22,"}]",CHAR(10)),"")</f>
@@ -4419,28 +4386,24 @@
       <c r="U23" s="30" t="str">
         <f aca="false">IF(AND(K23&lt;&gt;"",K23&lt;&gt;"+3v3",K23&lt;&gt;"GND"),CONCATENATE("set_property PACKAGE_PIN ",D23," [get_ports {",K23,"}]",CHAR(10),"set_property IOSTANDARD LVTTL [get_ports {",K23,"}]",CHAR(10)),"")</f>
         <v>set_property PACKAGE_PIN G18 [get_ports {ad_n31}]
-set_property IOSTANDARD LVTTL [get_ports {ad_n31}]
-</v>
+set_property IOSTANDARD LVTTL [get_ports {ad_n31}]</v>
       </c>
       <c r="V23" s="31" t="str">
         <f aca="false">IF(AND(K23&lt;&gt;"",K23&lt;&gt;"+3v3",K23&lt;&gt;"GND",NOT(ISNA(P23)),NOT(ISNA(N23))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S23/$V$8,"0.000")," [get_ports {",K23,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S23/$W$8,"0.000")," [get_ports {",K23,"}]",CHAR(10)),"")</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.237 [get_ports {ad_n31}]
-set_input_delay -clock clk_3v3_n -max 52.233 [get_ports {ad_n31}]
-</v>
+set_input_delay -clock clk_3v3_n -max 52.233 [get_ports {ad_n31}]</v>
       </c>
       <c r="W23" s="31" t="str">
         <f aca="false">IF(AND(K23&lt;&gt;"",K23&lt;&gt;"+3v3",K23&lt;&gt;"GND",NOT(ISNA(P23)),NOT(ISNA(N23))),CONCATENATE("set_output_delay -clock clk_3v3_n -min ",TEXT(-$W$6+P23/$V$8+$P$136/$V$8,"0.000")," [get_ports {",K23,"}]",CHAR(10),"set_output_delay -clock clk_3v3_n -max ",TEXT(0.25+0.25+$W$5+P23/$W$8+$P$136/$W$8,"0.000")," [get_ports {",K23,"}]",CHAR(10)),"")</f>
         <v>set_output_delay -clock clk_3v3_n -min -6.322 [get_ports {ad_n31}]
-set_output_delay -clock clk_3v3_n -max 53.404 [get_ports {ad_n31}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.404 [get_ports {ad_n31}]</v>
       </c>
       <c r="Y23" s="7" t="str">
         <f aca="false">CONCATENATE(IF(OR(T23="IO",T23="I"),V23,""),IF(OR(T23="IO",T23="O"),W23,""))</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.237 [get_ports {ad_n31}]
 set_input_delay -clock clk_3v3_n -max 52.233 [get_ports {ad_n31}]
 set_output_delay -clock clk_3v3_n -min -6.322 [get_ports {ad_n31}]
-set_output_delay -clock clk_3v3_n -max 53.404 [get_ports {ad_n31}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.404 [get_ports {ad_n31}]</v>
       </c>
       <c r="AG23" s="8" t="str">
         <f aca="false">IF(OR(LEFT(K23,3)="LED",LEFT(K23,16)="SBUS_DATA_OE_LED"),CONCATENATE("(",CHAR(34),"user_led",CHAR(34),", 0, Pins(",CHAR(34),D23,CHAR(34),"),  IOStandard(",CHAR(34),"lvcmos33",CHAR(34),")), ",CHAR(35),K23),"")</f>
@@ -4509,20 +4472,17 @@
       <c r="V24" s="31" t="str">
         <f aca="false">IF(AND(K24&lt;&gt;"",K24&lt;&gt;"+3v3",K24&lt;&gt;"GND",NOT(ISNA(P24)),NOT(ISNA(N24))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S24/$V$8,"0.000")," [get_ports {",K24,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S24/$W$8,"0.000")," [get_ports {",K24,"}]",CHAR(10)),"")</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.250 [get_ports {clk_n}]
-set_input_delay -clock clk_3v3_n -max 52.250 [get_ports {clk_n}]
-</v>
+set_input_delay -clock clk_3v3_n -max 52.250 [get_ports {clk_n}]</v>
       </c>
       <c r="W24" s="31" t="str">
         <f aca="false">IF(AND(K24&lt;&gt;"",K24&lt;&gt;"+3v3",K24&lt;&gt;"GND",NOT(ISNA(P24)),NOT(ISNA(N24))),CONCATENATE("set_output_delay -clock clk_3v3_n -min ",TEXT(-$W$6+P24/$V$8+$P$136/$V$8,"0.000")," [get_ports {",K24,"}]",CHAR(10),"set_output_delay -clock clk_3v3_n -max ",TEXT(0.25+0.25+$W$5+P24/$W$8+$P$136/$W$8,"0.000")," [get_ports {",K24,"}]",CHAR(10)),"")</f>
         <v>set_output_delay -clock clk_3v3_n -min -6.309 [get_ports {clk_n}]
-set_output_delay -clock clk_3v3_n -max 53.421 [get_ports {clk_n}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.421 [get_ports {clk_n}]</v>
       </c>
       <c r="Y24" s="32" t="str">
         <f aca="false">CONCATENATE(IF(OR(T24="IO",T24="I"),V24,""),IF(OR(T24="IO",T24="O"),W24,""))</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.250 [get_ports {clk_n}]
-set_input_delay -clock clk_3v3_n -max 52.250 [get_ports {clk_n}]
-</v>
+set_input_delay -clock clk_3v3_n -max 52.250 [get_ports {clk_n}]</v>
       </c>
       <c r="AG24" s="8" t="str">
         <f aca="false">IF(OR(LEFT(K24,3)="LED",LEFT(K24,16)="SBUS_DATA_OE_LED"),CONCATENATE("(",CHAR(34),"user_led",CHAR(34),", 0, Pins(",CHAR(34),D24,CHAR(34),"),  IOStandard(",CHAR(34),"lvcmos33",CHAR(34),")), ",CHAR(35),K24),"")</f>
@@ -4589,22 +4549,19 @@
       <c r="V25" s="31" t="str">
         <f aca="false">IF(AND(K25&lt;&gt;"",K25&lt;&gt;"+3v3",K25&lt;&gt;"GND",NOT(ISNA(P25)),NOT(ISNA(N25))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S25/$V$8,"0.000")," [get_ports {",K25,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S25/$W$8,"0.000")," [get_ports {",K25,"}]",CHAR(10)),"")</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.229 [get_ports {ad_n29}]
-set_input_delay -clock clk_3v3_n -max 52.221 [get_ports {ad_n29}]
-</v>
+set_input_delay -clock clk_3v3_n -max 52.221 [get_ports {ad_n29}]</v>
       </c>
       <c r="W25" s="31" t="str">
         <f aca="false">IF(AND(K25&lt;&gt;"",K25&lt;&gt;"+3v3",K25&lt;&gt;"GND",NOT(ISNA(P25)),NOT(ISNA(N25))),CONCATENATE("set_output_delay -clock clk_3v3_n -min ",TEXT(-$W$6+P25/$V$8+$P$136/$V$8,"0.000")," [get_ports {",K25,"}]",CHAR(10),"set_output_delay -clock clk_3v3_n -max ",TEXT(0.25+0.25+$W$5+P25/$W$8+$P$136/$W$8,"0.000")," [get_ports {",K25,"}]",CHAR(10)),"")</f>
         <v>set_output_delay -clock clk_3v3_n -min -6.330 [get_ports {ad_n29}]
-set_output_delay -clock clk_3v3_n -max 53.393 [get_ports {ad_n29}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.393 [get_ports {ad_n29}]</v>
       </c>
       <c r="Y25" s="7" t="str">
         <f aca="false">CONCATENATE(IF(OR(T25="IO",T25="I"),V25,""),IF(OR(T25="IO",T25="O"),W25,""))</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.229 [get_ports {ad_n29}]
 set_input_delay -clock clk_3v3_n -max 52.221 [get_ports {ad_n29}]
 set_output_delay -clock clk_3v3_n -min -6.330 [get_ports {ad_n29}]
-set_output_delay -clock clk_3v3_n -max 53.393 [get_ports {ad_n29}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.393 [get_ports {ad_n29}]</v>
       </c>
       <c r="AG25" s="8" t="str">
         <f aca="false">IF(OR(LEFT(K25,3)="LED",LEFT(K25,16)="SBUS_DATA_OE_LED"),CONCATENATE("(",CHAR(34),"user_led",CHAR(34),", 0, Pins(",CHAR(34),D25,CHAR(34),"),  IOStandard(",CHAR(34),"lvcmos33",CHAR(34),")), ",CHAR(35),K25),"")</f>
@@ -4673,22 +4630,19 @@
       <c r="V26" s="31" t="str">
         <f aca="false">IF(AND(K26&lt;&gt;"",K26&lt;&gt;"+3v3",K26&lt;&gt;"GND",NOT(ISNA(P26)),NOT(ISNA(N26))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S26/$V$8,"0.000")," [get_ports {",K26,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S26/$W$8,"0.000")," [get_ports {",K26,"}]",CHAR(10)),"")</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.282 [get_ports {ad_n30}]
-set_input_delay -clock clk_3v3_n -max 52.293 [get_ports {ad_n30}]
-</v>
+set_input_delay -clock clk_3v3_n -max 52.293 [get_ports {ad_n30}]</v>
       </c>
       <c r="W26" s="31" t="str">
         <f aca="false">IF(AND(K26&lt;&gt;"",K26&lt;&gt;"+3v3",K26&lt;&gt;"GND",NOT(ISNA(P26)),NOT(ISNA(N26))),CONCATENATE("set_output_delay -clock clk_3v3_n -min ",TEXT(-$W$6+P26/$V$8+$P$136/$V$8,"0.000")," [get_ports {",K26,"}]",CHAR(10),"set_output_delay -clock clk_3v3_n -max ",TEXT(0.25+0.25+$W$5+P26/$W$8+$P$136/$W$8,"0.000")," [get_ports {",K26,"}]",CHAR(10)),"")</f>
         <v>set_output_delay -clock clk_3v3_n -min -6.277 [get_ports {ad_n30}]
-set_output_delay -clock clk_3v3_n -max 53.464 [get_ports {ad_n30}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.464 [get_ports {ad_n30}]</v>
       </c>
       <c r="Y26" s="7" t="str">
         <f aca="false">CONCATENATE(IF(OR(T26="IO",T26="I"),V26,""),IF(OR(T26="IO",T26="O"),W26,""))</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.282 [get_ports {ad_n30}]
 set_input_delay -clock clk_3v3_n -max 52.293 [get_ports {ad_n30}]
 set_output_delay -clock clk_3v3_n -min -6.277 [get_ports {ad_n30}]
-set_output_delay -clock clk_3v3_n -max 53.464 [get_ports {ad_n30}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.464 [get_ports {ad_n30}]</v>
       </c>
       <c r="AG26" s="8" t="str">
         <f aca="false">IF(OR(LEFT(K26,3)="LED",LEFT(K26,16)="SBUS_DATA_OE_LED"),CONCATENATE("(",CHAR(34),"user_led",CHAR(34),", 0, Pins(",CHAR(34),D26,CHAR(34),"),  IOStandard(",CHAR(34),"lvcmos33",CHAR(34),")), ",CHAR(35),K26),"")</f>
@@ -4755,22 +4709,19 @@
       <c r="V27" s="31" t="str">
         <f aca="false">IF(AND(K27&lt;&gt;"",K27&lt;&gt;"+3v3",K27&lt;&gt;"GND",NOT(ISNA(P27)),NOT(ISNA(N27))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S27/$V$8,"0.000")," [get_ports {",K27,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S27/$W$8,"0.000")," [get_ports {",K27,"}]",CHAR(10)),"")</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.224 [get_ports {ad_n27}]
-set_input_delay -clock clk_3v3_n -max 52.215 [get_ports {ad_n27}]
-</v>
+set_input_delay -clock clk_3v3_n -max 52.215 [get_ports {ad_n27}]</v>
       </c>
       <c r="W27" s="31" t="str">
         <f aca="false">IF(AND(K27&lt;&gt;"",K27&lt;&gt;"+3v3",K27&lt;&gt;"GND",NOT(ISNA(P27)),NOT(ISNA(N27))),CONCATENATE("set_output_delay -clock clk_3v3_n -min ",TEXT(-$W$6+P27/$V$8+$P$136/$V$8,"0.000")," [get_ports {",K27,"}]",CHAR(10),"set_output_delay -clock clk_3v3_n -max ",TEXT(0.25+0.25+$W$5+P27/$W$8+$P$136/$W$8,"0.000")," [get_ports {",K27,"}]",CHAR(10)),"")</f>
         <v>set_output_delay -clock clk_3v3_n -min -6.335 [get_ports {ad_n27}]
-set_output_delay -clock clk_3v3_n -max 53.386 [get_ports {ad_n27}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.386 [get_ports {ad_n27}]</v>
       </c>
       <c r="Y27" s="7" t="str">
         <f aca="false">CONCATENATE(IF(OR(T27="IO",T27="I"),V27,""),IF(OR(T27="IO",T27="O"),W27,""))</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.224 [get_ports {ad_n27}]
 set_input_delay -clock clk_3v3_n -max 52.215 [get_ports {ad_n27}]
 set_output_delay -clock clk_3v3_n -min -6.335 [get_ports {ad_n27}]
-set_output_delay -clock clk_3v3_n -max 53.386 [get_ports {ad_n27}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.386 [get_ports {ad_n27}]</v>
       </c>
       <c r="AG27" s="8" t="str">
         <f aca="false">IF(OR(LEFT(K27,3)="LED",LEFT(K27,16)="SBUS_DATA_OE_LED"),CONCATENATE("(",CHAR(34),"user_led",CHAR(34),", 0, Pins(",CHAR(34),D27,CHAR(34),"),  IOStandard(",CHAR(34),"lvcmos33",CHAR(34),")), ",CHAR(35),K27),"")</f>
@@ -4839,22 +4790,19 @@
       <c r="V28" s="31" t="str">
         <f aca="false">IF(AND(K28&lt;&gt;"",K28&lt;&gt;"+3v3",K28&lt;&gt;"GND",NOT(ISNA(P28)),NOT(ISNA(N28))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S28/$V$8,"0.000")," [get_ports {",K28,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S28/$W$8,"0.000")," [get_ports {",K28,"}]",CHAR(10)),"")</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.202 [get_ports {ad_n28}]
-set_input_delay -clock clk_3v3_n -max 52.186 [get_ports {ad_n28}]
-</v>
+set_input_delay -clock clk_3v3_n -max 52.186 [get_ports {ad_n28}]</v>
       </c>
       <c r="W28" s="31" t="str">
         <f aca="false">IF(AND(K28&lt;&gt;"",K28&lt;&gt;"+3v3",K28&lt;&gt;"GND",NOT(ISNA(P28)),NOT(ISNA(N28))),CONCATENATE("set_output_delay -clock clk_3v3_n -min ",TEXT(-$W$6+P28/$V$8+$P$136/$V$8,"0.000")," [get_ports {",K28,"}]",CHAR(10),"set_output_delay -clock clk_3v3_n -max ",TEXT(0.25+0.25+$W$5+P28/$W$8+$P$136/$W$8,"0.000")," [get_ports {",K28,"}]",CHAR(10)),"")</f>
         <v>set_output_delay -clock clk_3v3_n -min -6.357 [get_ports {ad_n28}]
-set_output_delay -clock clk_3v3_n -max 53.357 [get_ports {ad_n28}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.357 [get_ports {ad_n28}]</v>
       </c>
       <c r="Y28" s="7" t="str">
         <f aca="false">CONCATENATE(IF(OR(T28="IO",T28="I"),V28,""),IF(OR(T28="IO",T28="O"),W28,""))</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.202 [get_ports {ad_n28}]
 set_input_delay -clock clk_3v3_n -max 52.186 [get_ports {ad_n28}]
 set_output_delay -clock clk_3v3_n -min -6.357 [get_ports {ad_n28}]
-set_output_delay -clock clk_3v3_n -max 53.357 [get_ports {ad_n28}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.357 [get_ports {ad_n28}]</v>
       </c>
       <c r="AG28" s="8" t="str">
         <f aca="false">IF(OR(LEFT(K28,3)="LED",LEFT(K28,16)="SBUS_DATA_OE_LED"),CONCATENATE("(",CHAR(34),"user_led",CHAR(34),", 0, Pins(",CHAR(34),D28,CHAR(34),"),  IOStandard(",CHAR(34),"lvcmos33",CHAR(34),")), ",CHAR(35),K28),"")</f>
@@ -4921,22 +4869,19 @@
       <c r="V29" s="31" t="str">
         <f aca="false">IF(AND(K29&lt;&gt;"",K29&lt;&gt;"+3v3",K29&lt;&gt;"GND",NOT(ISNA(P29)),NOT(ISNA(N29))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S29/$V$8,"0.000")," [get_ports {",K29,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S29/$W$8,"0.000")," [get_ports {",K29,"}]",CHAR(10)),"")</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.214 [get_ports {ad_n25}]
-set_input_delay -clock clk_3v3_n -max 52.202 [get_ports {ad_n25}]
-</v>
+set_input_delay -clock clk_3v3_n -max 52.202 [get_ports {ad_n25}]</v>
       </c>
       <c r="W29" s="31" t="str">
         <f aca="false">IF(AND(K29&lt;&gt;"",K29&lt;&gt;"+3v3",K29&lt;&gt;"GND",NOT(ISNA(P29)),NOT(ISNA(N29))),CONCATENATE("set_output_delay -clock clk_3v3_n -min ",TEXT(-$W$6+P29/$V$8+$P$136/$V$8,"0.000")," [get_ports {",K29,"}]",CHAR(10),"set_output_delay -clock clk_3v3_n -max ",TEXT(0.25+0.25+$W$5+P29/$W$8+$P$136/$W$8,"0.000")," [get_ports {",K29,"}]",CHAR(10)),"")</f>
         <v>set_output_delay -clock clk_3v3_n -min -6.345 [get_ports {ad_n25}]
-set_output_delay -clock clk_3v3_n -max 53.374 [get_ports {ad_n25}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.374 [get_ports {ad_n25}]</v>
       </c>
       <c r="Y29" s="7" t="str">
         <f aca="false">CONCATENATE(IF(OR(T29="IO",T29="I"),V29,""),IF(OR(T29="IO",T29="O"),W29,""))</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.214 [get_ports {ad_n25}]
 set_input_delay -clock clk_3v3_n -max 52.202 [get_ports {ad_n25}]
 set_output_delay -clock clk_3v3_n -min -6.345 [get_ports {ad_n25}]
-set_output_delay -clock clk_3v3_n -max 53.374 [get_ports {ad_n25}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.374 [get_ports {ad_n25}]</v>
       </c>
       <c r="AG29" s="8" t="str">
         <f aca="false">IF(OR(LEFT(K29,3)="LED",LEFT(K29,16)="SBUS_DATA_OE_LED"),CONCATENATE("(",CHAR(34),"user_led",CHAR(34),", 0, Pins(",CHAR(34),D29,CHAR(34),"),  IOStandard(",CHAR(34),"lvcmos33",CHAR(34),")), ",CHAR(35),K29),"")</f>
@@ -5003,22 +4948,19 @@
       <c r="V30" s="31" t="str">
         <f aca="false">IF(AND(K30&lt;&gt;"",K30&lt;&gt;"+3v3",K30&lt;&gt;"GND",NOT(ISNA(P30)),NOT(ISNA(N30))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S30/$V$8,"0.000")," [get_ports {",K30,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S30/$W$8,"0.000")," [get_ports {",K30,"}]",CHAR(10)),"")</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.189 [get_ports {ad_n26}]
-set_input_delay -clock clk_3v3_n -max 52.169 [get_ports {ad_n26}]
-</v>
+set_input_delay -clock clk_3v3_n -max 52.169 [get_ports {ad_n26}]</v>
       </c>
       <c r="W30" s="31" t="str">
         <f aca="false">IF(AND(K30&lt;&gt;"",K30&lt;&gt;"+3v3",K30&lt;&gt;"GND",NOT(ISNA(P30)),NOT(ISNA(N30))),CONCATENATE("set_output_delay -clock clk_3v3_n -min ",TEXT(-$W$6+P30/$V$8+$P$136/$V$8,"0.000")," [get_ports {",K30,"}]",CHAR(10),"set_output_delay -clock clk_3v3_n -max ",TEXT(0.25+0.25+$W$5+P30/$W$8+$P$136/$W$8,"0.000")," [get_ports {",K30,"}]",CHAR(10)),"")</f>
         <v>set_output_delay -clock clk_3v3_n -min -6.370 [get_ports {ad_n26}]
-set_output_delay -clock clk_3v3_n -max 53.340 [get_ports {ad_n26}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.340 [get_ports {ad_n26}]</v>
       </c>
       <c r="Y30" s="7" t="str">
         <f aca="false">CONCATENATE(IF(OR(T30="IO",T30="I"),V30,""),IF(OR(T30="IO",T30="O"),W30,""))</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.189 [get_ports {ad_n26}]
 set_input_delay -clock clk_3v3_n -max 52.169 [get_ports {ad_n26}]
 set_output_delay -clock clk_3v3_n -min -6.370 [get_ports {ad_n26}]
-set_output_delay -clock clk_3v3_n -max 53.340 [get_ports {ad_n26}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.340 [get_ports {ad_n26}]</v>
       </c>
       <c r="AG30" s="8" t="str">
         <f aca="false">IF(OR(LEFT(K30,3)="LED",LEFT(K30,16)="SBUS_DATA_OE_LED"),CONCATENATE("(",CHAR(34),"user_led",CHAR(34),", 0, Pins(",CHAR(34),D30,CHAR(34),"),  IOStandard(",CHAR(34),"lvcmos33",CHAR(34),")), ",CHAR(35),K30),"")</f>
@@ -5159,22 +5101,19 @@
       <c r="V32" s="31" t="str">
         <f aca="false">IF(AND(K32&lt;&gt;"",K32&lt;&gt;"+3v3",K32&lt;&gt;"GND",NOT(ISNA(P32)),NOT(ISNA(N32))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S32/$V$8,"0.000")," [get_ports {",K32,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S32/$W$8,"0.000")," [get_ports {",K32,"}]",CHAR(10)),"")</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.185 [get_ports {ad_n24}]
-set_input_delay -clock clk_3v3_n -max 52.163 [get_ports {ad_n24}]
-</v>
+set_input_delay -clock clk_3v3_n -max 52.163 [get_ports {ad_n24}]</v>
       </c>
       <c r="W32" s="31" t="str">
         <f aca="false">IF(AND(K32&lt;&gt;"",K32&lt;&gt;"+3v3",K32&lt;&gt;"GND",NOT(ISNA(P32)),NOT(ISNA(N32))),CONCATENATE("set_output_delay -clock clk_3v3_n -min ",TEXT(-$W$6+P32/$V$8+$P$136/$V$8,"0.000")," [get_ports {",K32,"}]",CHAR(10),"set_output_delay -clock clk_3v3_n -max ",TEXT(0.25+0.25+$W$5+P32/$W$8+$P$136/$W$8,"0.000")," [get_ports {",K32,"}]",CHAR(10)),"")</f>
         <v>set_output_delay -clock clk_3v3_n -min -6.374 [get_ports {ad_n24}]
-set_output_delay -clock clk_3v3_n -max 53.335 [get_ports {ad_n24}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.335 [get_ports {ad_n24}]</v>
       </c>
       <c r="Y32" s="7" t="str">
         <f aca="false">CONCATENATE(IF(OR(T32="IO",T32="I"),V32,""),IF(OR(T32="IO",T32="O"),W32,""))</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.185 [get_ports {ad_n24}]
 set_input_delay -clock clk_3v3_n -max 52.163 [get_ports {ad_n24}]
 set_output_delay -clock clk_3v3_n -min -6.374 [get_ports {ad_n24}]
-set_output_delay -clock clk_3v3_n -max 53.335 [get_ports {ad_n24}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.335 [get_ports {ad_n24}]</v>
       </c>
       <c r="AG32" s="8" t="str">
         <f aca="false">IF(OR(LEFT(K32,3)="LED",LEFT(K32,16)="SBUS_DATA_OE_LED"),CONCATENATE("(",CHAR(34),"user_led",CHAR(34),", 0, Pins(",CHAR(34),D32,CHAR(34),"),  IOStandard(",CHAR(34),"lvcmos33",CHAR(34),")), ",CHAR(35),K32),"")</f>
@@ -5597,22 +5536,19 @@
       <c r="V39" s="31" t="str">
         <f aca="false">IF(AND(K39&lt;&gt;"",K39&lt;&gt;"+3v3",K39&lt;&gt;"GND",NOT(ISNA(P39)),NOT(ISNA(N39))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S39/$V$8,"0.000")," [get_ports {",K39,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S39/$W$8,"0.000")," [get_ports {",K39,"}]",CHAR(10)),"")</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.192 [get_ports {ad_n23}]
-set_input_delay -clock clk_3v3_n -max 52.173 [get_ports {ad_n23}]
-</v>
+set_input_delay -clock clk_3v3_n -max 52.173 [get_ports {ad_n23}]</v>
       </c>
       <c r="W39" s="31" t="str">
         <f aca="false">IF(AND(K39&lt;&gt;"",K39&lt;&gt;"+3v3",K39&lt;&gt;"GND",NOT(ISNA(P39)),NOT(ISNA(N39))),CONCATENATE("set_output_delay -clock clk_3v3_n -min ",TEXT(-$W$6+P39/$V$8+$P$136/$V$8,"0.000")," [get_ports {",K39,"}]",CHAR(10),"set_output_delay -clock clk_3v3_n -max ",TEXT(0.25+0.25+$W$5+P39/$W$8+$P$136/$W$8,"0.000")," [get_ports {",K39,"}]",CHAR(10)),"")</f>
         <v>set_output_delay -clock clk_3v3_n -min -6.367 [get_ports {ad_n23}]
-set_output_delay -clock clk_3v3_n -max 53.344 [get_ports {ad_n23}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.344 [get_ports {ad_n23}]</v>
       </c>
       <c r="Y39" s="7" t="str">
         <f aca="false">CONCATENATE(IF(OR(T39="IO",T39="I"),V39,""),IF(OR(T39="IO",T39="O"),W39,""))</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.192 [get_ports {ad_n23}]
 set_input_delay -clock clk_3v3_n -max 52.173 [get_ports {ad_n23}]
 set_output_delay -clock clk_3v3_n -min -6.367 [get_ports {ad_n23}]
-set_output_delay -clock clk_3v3_n -max 53.344 [get_ports {ad_n23}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.344 [get_ports {ad_n23}]</v>
       </c>
       <c r="AG39" s="8" t="str">
         <f aca="false">IF(OR(LEFT(K39,3)="LED",LEFT(K39,16)="SBUS_DATA_OE_LED"),CONCATENATE("(",CHAR(34),"user_led",CHAR(34),", 0, Pins(",CHAR(34),D39,CHAR(34),"),  IOStandard(",CHAR(34),"lvcmos33",CHAR(34),")), ",CHAR(35),K39),"")</f>
@@ -5679,22 +5615,19 @@
       <c r="V40" s="31" t="str">
         <f aca="false">IF(AND(K40&lt;&gt;"",K40&lt;&gt;"+3v3",K40&lt;&gt;"GND",NOT(ISNA(P40)),NOT(ISNA(N40))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S40/$V$8,"0.000")," [get_ports {",K40,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S40/$W$8,"0.000")," [get_ports {",K40,"}]",CHAR(10)),"")</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.149 [get_ports {ad_n22}]
-set_input_delay -clock clk_3v3_n -max 52.115 [get_ports {ad_n22}]
-</v>
+set_input_delay -clock clk_3v3_n -max 52.115 [get_ports {ad_n22}]</v>
       </c>
       <c r="W40" s="31" t="str">
         <f aca="false">IF(AND(K40&lt;&gt;"",K40&lt;&gt;"+3v3",K40&lt;&gt;"GND",NOT(ISNA(P40)),NOT(ISNA(N40))),CONCATENATE("set_output_delay -clock clk_3v3_n -min ",TEXT(-$W$6+P40/$V$8+$P$136/$V$8,"0.000")," [get_ports {",K40,"}]",CHAR(10),"set_output_delay -clock clk_3v3_n -max ",TEXT(0.25+0.25+$W$5+P40/$W$8+$P$136/$W$8,"0.000")," [get_ports {",K40,"}]",CHAR(10)),"")</f>
         <v>set_output_delay -clock clk_3v3_n -min -6.410 [get_ports {ad_n22}]
-set_output_delay -clock clk_3v3_n -max 53.286 [get_ports {ad_n22}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.286 [get_ports {ad_n22}]</v>
       </c>
       <c r="Y40" s="7" t="str">
         <f aca="false">CONCATENATE(IF(OR(T40="IO",T40="I"),V40,""),IF(OR(T40="IO",T40="O"),W40,""))</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.149 [get_ports {ad_n22}]
 set_input_delay -clock clk_3v3_n -max 52.115 [get_ports {ad_n22}]
 set_output_delay -clock clk_3v3_n -min -6.410 [get_ports {ad_n22}]
-set_output_delay -clock clk_3v3_n -max 53.286 [get_ports {ad_n22}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.286 [get_ports {ad_n22}]</v>
       </c>
       <c r="AG40" s="8" t="str">
         <f aca="false">IF(OR(LEFT(K40,3)="LED",LEFT(K40,16)="SBUS_DATA_OE_LED"),CONCATENATE("(",CHAR(34),"user_led",CHAR(34),", 0, Pins(",CHAR(34),D40,CHAR(34),"),  IOStandard(",CHAR(34),"lvcmos33",CHAR(34),")), ",CHAR(35),K40),"")</f>
@@ -5763,22 +5696,19 @@
       <c r="V41" s="31" t="str">
         <f aca="false">IF(AND(K41&lt;&gt;"",K41&lt;&gt;"+3v3",K41&lt;&gt;"GND",NOT(ISNA(P41)),NOT(ISNA(N41))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S41/$V$8,"0.000")," [get_ports {",K41,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S41/$W$8,"0.000")," [get_ports {",K41,"}]",CHAR(10)),"")</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.177 [get_ports {ad_n21}]
-set_input_delay -clock clk_3v3_n -max 52.152 [get_ports {ad_n21}]
-</v>
+set_input_delay -clock clk_3v3_n -max 52.152 [get_ports {ad_n21}]</v>
       </c>
       <c r="W41" s="31" t="str">
         <f aca="false">IF(AND(K41&lt;&gt;"",K41&lt;&gt;"+3v3",K41&lt;&gt;"GND",NOT(ISNA(P41)),NOT(ISNA(N41))),CONCATENATE("set_output_delay -clock clk_3v3_n -min ",TEXT(-$W$6+P41/$V$8+$P$136/$V$8,"0.000")," [get_ports {",K41,"}]",CHAR(10),"set_output_delay -clock clk_3v3_n -max ",TEXT(0.25+0.25+$W$5+P41/$W$8+$P$136/$W$8,"0.000")," [get_ports {",K41,"}]",CHAR(10)),"")</f>
         <v>set_output_delay -clock clk_3v3_n -min -6.382 [get_ports {ad_n21}]
-set_output_delay -clock clk_3v3_n -max 53.324 [get_ports {ad_n21}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.324 [get_ports {ad_n21}]</v>
       </c>
       <c r="Y41" s="7" t="str">
         <f aca="false">CONCATENATE(IF(OR(T41="IO",T41="I"),V41,""),IF(OR(T41="IO",T41="O"),W41,""))</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.177 [get_ports {ad_n21}]
 set_input_delay -clock clk_3v3_n -max 52.152 [get_ports {ad_n21}]
 set_output_delay -clock clk_3v3_n -min -6.382 [get_ports {ad_n21}]
-set_output_delay -clock clk_3v3_n -max 53.324 [get_ports {ad_n21}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.324 [get_ports {ad_n21}]</v>
       </c>
       <c r="AG41" s="8" t="str">
         <f aca="false">IF(OR(LEFT(K41,3)="LED",LEFT(K41,16)="SBUS_DATA_OE_LED"),CONCATENATE("(",CHAR(34),"user_led",CHAR(34),", 0, Pins(",CHAR(34),D41,CHAR(34),"),  IOStandard(",CHAR(34),"lvcmos33",CHAR(34),")), ",CHAR(35),K41),"")</f>
@@ -5847,22 +5777,19 @@
       <c r="V42" s="31" t="str">
         <f aca="false">IF(AND(K42&lt;&gt;"",K42&lt;&gt;"+3v3",K42&lt;&gt;"GND",NOT(ISNA(P42)),NOT(ISNA(N42))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S42/$V$8,"0.000")," [get_ports {",K42,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S42/$W$8,"0.000")," [get_ports {",K42,"}]",CHAR(10)),"")</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.136 [get_ports {ad_n20}]
-set_input_delay -clock clk_3v3_n -max 52.098 [get_ports {ad_n20}]
-</v>
+set_input_delay -clock clk_3v3_n -max 52.098 [get_ports {ad_n20}]</v>
       </c>
       <c r="W42" s="31" t="str">
         <f aca="false">IF(AND(K42&lt;&gt;"",K42&lt;&gt;"+3v3",K42&lt;&gt;"GND",NOT(ISNA(P42)),NOT(ISNA(N42))),CONCATENATE("set_output_delay -clock clk_3v3_n -min ",TEXT(-$W$6+P42/$V$8+$P$136/$V$8,"0.000")," [get_ports {",K42,"}]",CHAR(10),"set_output_delay -clock clk_3v3_n -max ",TEXT(0.25+0.25+$W$5+P42/$W$8+$P$136/$W$8,"0.000")," [get_ports {",K42,"}]",CHAR(10)),"")</f>
         <v>set_output_delay -clock clk_3v3_n -min -6.423 [get_ports {ad_n20}]
-set_output_delay -clock clk_3v3_n -max 53.270 [get_ports {ad_n20}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.270 [get_ports {ad_n20}]</v>
       </c>
       <c r="Y42" s="7" t="str">
         <f aca="false">CONCATENATE(IF(OR(T42="IO",T42="I"),V42,""),IF(OR(T42="IO",T42="O"),W42,""))</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.136 [get_ports {ad_n20}]
 set_input_delay -clock clk_3v3_n -max 52.098 [get_ports {ad_n20}]
 set_output_delay -clock clk_3v3_n -min -6.423 [get_ports {ad_n20}]
-set_output_delay -clock clk_3v3_n -max 53.270 [get_ports {ad_n20}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.270 [get_ports {ad_n20}]</v>
       </c>
       <c r="AG42" s="8" t="str">
         <f aca="false">IF(OR(LEFT(K42,3)="LED",LEFT(K42,16)="SBUS_DATA_OE_LED"),CONCATENATE("(",CHAR(34),"user_led",CHAR(34),", 0, Pins(",CHAR(34),D42,CHAR(34),"),  IOStandard(",CHAR(34),"lvcmos33",CHAR(34),")), ",CHAR(35),K42),"")</f>
@@ -5929,22 +5856,19 @@
       <c r="V43" s="31" t="str">
         <f aca="false">IF(AND(K43&lt;&gt;"",K43&lt;&gt;"+3v3",K43&lt;&gt;"GND",NOT(ISNA(P43)),NOT(ISNA(N43))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S43/$V$8,"0.000")," [get_ports {",K43,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S43/$W$8,"0.000")," [get_ports {",K43,"}]",CHAR(10)),"")</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.159 [get_ports {ad_n19}]
-set_input_delay -clock clk_3v3_n -max 52.129 [get_ports {ad_n19}]
-</v>
+set_input_delay -clock clk_3v3_n -max 52.129 [get_ports {ad_n19}]</v>
       </c>
       <c r="W43" s="31" t="str">
         <f aca="false">IF(AND(K43&lt;&gt;"",K43&lt;&gt;"+3v3",K43&lt;&gt;"GND",NOT(ISNA(P43)),NOT(ISNA(N43))),CONCATENATE("set_output_delay -clock clk_3v3_n -min ",TEXT(-$W$6+P43/$V$8+$P$136/$V$8,"0.000")," [get_ports {",K43,"}]",CHAR(10),"set_output_delay -clock clk_3v3_n -max ",TEXT(0.25+0.25+$W$5+P43/$W$8+$P$136/$W$8,"0.000")," [get_ports {",K43,"}]",CHAR(10)),"")</f>
         <v>set_output_delay -clock clk_3v3_n -min -6.400 [get_ports {ad_n19}]
-set_output_delay -clock clk_3v3_n -max 53.300 [get_ports {ad_n19}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.300 [get_ports {ad_n19}]</v>
       </c>
       <c r="Y43" s="7" t="str">
         <f aca="false">CONCATENATE(IF(OR(T43="IO",T43="I"),V43,""),IF(OR(T43="IO",T43="O"),W43,""))</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.159 [get_ports {ad_n19}]
 set_input_delay -clock clk_3v3_n -max 52.129 [get_ports {ad_n19}]
 set_output_delay -clock clk_3v3_n -min -6.400 [get_ports {ad_n19}]
-set_output_delay -clock clk_3v3_n -max 53.300 [get_ports {ad_n19}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.300 [get_ports {ad_n19}]</v>
       </c>
       <c r="AG43" s="8" t="str">
         <f aca="false">IF(OR(LEFT(K43,3)="LED",LEFT(K43,16)="SBUS_DATA_OE_LED"),CONCATENATE("(",CHAR(34),"user_led",CHAR(34),", 0, Pins(",CHAR(34),D43,CHAR(34),"),  IOStandard(",CHAR(34),"lvcmos33",CHAR(34),")), ",CHAR(35),K43),"")</f>
@@ -6011,22 +5935,19 @@
       <c r="V44" s="31" t="str">
         <f aca="false">IF(AND(K44&lt;&gt;"",K44&lt;&gt;"+3v3",K44&lt;&gt;"GND",NOT(ISNA(P44)),NOT(ISNA(N44))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S44/$V$8,"0.000")," [get_ports {",K44,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S44/$W$8,"0.000")," [get_ports {",K44,"}]",CHAR(10)),"")</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.123 [get_ports {ad_n18}]
-set_input_delay -clock clk_3v3_n -max 52.080 [get_ports {ad_n18}]
-</v>
+set_input_delay -clock clk_3v3_n -max 52.080 [get_ports {ad_n18}]</v>
       </c>
       <c r="W44" s="31" t="str">
         <f aca="false">IF(AND(K44&lt;&gt;"",K44&lt;&gt;"+3v3",K44&lt;&gt;"GND",NOT(ISNA(P44)),NOT(ISNA(N44))),CONCATENATE("set_output_delay -clock clk_3v3_n -min ",TEXT(-$W$6+P44/$V$8+$P$136/$V$8,"0.000")," [get_ports {",K44,"}]",CHAR(10),"set_output_delay -clock clk_3v3_n -max ",TEXT(0.25+0.25+$W$5+P44/$W$8+$P$136/$W$8,"0.000")," [get_ports {",K44,"}]",CHAR(10)),"")</f>
         <v>set_output_delay -clock clk_3v3_n -min -6.436 [get_ports {ad_n18}]
-set_output_delay -clock clk_3v3_n -max 53.252 [get_ports {ad_n18}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.252 [get_ports {ad_n18}]</v>
       </c>
       <c r="Y44" s="7" t="str">
         <f aca="false">CONCATENATE(IF(OR(T44="IO",T44="I"),V44,""),IF(OR(T44="IO",T44="O"),W44,""))</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.123 [get_ports {ad_n18}]
 set_input_delay -clock clk_3v3_n -max 52.080 [get_ports {ad_n18}]
 set_output_delay -clock clk_3v3_n -min -6.436 [get_ports {ad_n18}]
-set_output_delay -clock clk_3v3_n -max 53.252 [get_ports {ad_n18}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.252 [get_ports {ad_n18}]</v>
       </c>
       <c r="AG44" s="8" t="str">
         <f aca="false">IF(OR(LEFT(K44,3)="LED",LEFT(K44,16)="SBUS_DATA_OE_LED"),CONCATENATE("(",CHAR(34),"user_led",CHAR(34),", 0, Pins(",CHAR(34),D44,CHAR(34),"),  IOStandard(",CHAR(34),"lvcmos33",CHAR(34),")), ",CHAR(35),K44),"")</f>
@@ -6095,22 +6016,19 @@
       <c r="V45" s="31" t="str">
         <f aca="false">IF(AND(K45&lt;&gt;"",K45&lt;&gt;"+3v3",K45&lt;&gt;"GND",NOT(ISNA(P45)),NOT(ISNA(N45))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S45/$V$8,"0.000")," [get_ports {",K45,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S45/$W$8,"0.000")," [get_ports {",K45,"}]",CHAR(10)),"")</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.155 [get_ports {ad_n17}]
-set_input_delay -clock clk_3v3_n -max 52.123 [get_ports {ad_n17}]
-</v>
+set_input_delay -clock clk_3v3_n -max 52.123 [get_ports {ad_n17}]</v>
       </c>
       <c r="W45" s="31" t="str">
         <f aca="false">IF(AND(K45&lt;&gt;"",K45&lt;&gt;"+3v3",K45&lt;&gt;"GND",NOT(ISNA(P45)),NOT(ISNA(N45))),CONCATENATE("set_output_delay -clock clk_3v3_n -min ",TEXT(-$W$6+P45/$V$8+$P$136/$V$8,"0.000")," [get_ports {",K45,"}]",CHAR(10),"set_output_delay -clock clk_3v3_n -max ",TEXT(0.25+0.25+$W$5+P45/$W$8+$P$136/$W$8,"0.000")," [get_ports {",K45,"}]",CHAR(10)),"")</f>
         <v>set_output_delay -clock clk_3v3_n -min -6.404 [get_ports {ad_n17}]
-set_output_delay -clock clk_3v3_n -max 53.294 [get_ports {ad_n17}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.294 [get_ports {ad_n17}]</v>
       </c>
       <c r="Y45" s="7" t="str">
         <f aca="false">CONCATENATE(IF(OR(T45="IO",T45="I"),V45,""),IF(OR(T45="IO",T45="O"),W45,""))</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.155 [get_ports {ad_n17}]
 set_input_delay -clock clk_3v3_n -max 52.123 [get_ports {ad_n17}]
 set_output_delay -clock clk_3v3_n -min -6.404 [get_ports {ad_n17}]
-set_output_delay -clock clk_3v3_n -max 53.294 [get_ports {ad_n17}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.294 [get_ports {ad_n17}]</v>
       </c>
       <c r="AG45" s="8" t="str">
         <f aca="false">IF(OR(LEFT(K45,3)="LED",LEFT(K45,16)="SBUS_DATA_OE_LED"),CONCATENATE("(",CHAR(34),"user_led",CHAR(34),", 0, Pins(",CHAR(34),D45,CHAR(34),"),  IOStandard(",CHAR(34),"lvcmos33",CHAR(34),")), ",CHAR(35),K45),"")</f>
@@ -6177,22 +6095,19 @@
       <c r="V46" s="31" t="str">
         <f aca="false">IF(AND(K46&lt;&gt;"",K46&lt;&gt;"+3v3",K46&lt;&gt;"GND",NOT(ISNA(P46)),NOT(ISNA(N46))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S46/$V$8,"0.000")," [get_ports {",K46,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S46/$W$8,"0.000")," [get_ports {",K46,"}]",CHAR(10)),"")</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.109 [get_ports {ad_n16}]
-set_input_delay -clock clk_3v3_n -max 52.062 [get_ports {ad_n16}]
-</v>
+set_input_delay -clock clk_3v3_n -max 52.062 [get_ports {ad_n16}]</v>
       </c>
       <c r="W46" s="31" t="str">
         <f aca="false">IF(AND(K46&lt;&gt;"",K46&lt;&gt;"+3v3",K46&lt;&gt;"GND",NOT(ISNA(P46)),NOT(ISNA(N46))),CONCATENATE("set_output_delay -clock clk_3v3_n -min ",TEXT(-$W$6+P46/$V$8+$P$136/$V$8,"0.000")," [get_ports {",K46,"}]",CHAR(10),"set_output_delay -clock clk_3v3_n -max ",TEXT(0.25+0.25+$W$5+P46/$W$8+$P$136/$W$8,"0.000")," [get_ports {",K46,"}]",CHAR(10)),"")</f>
         <v>set_output_delay -clock clk_3v3_n -min -6.450 [get_ports {ad_n16}]
-set_output_delay -clock clk_3v3_n -max 53.233 [get_ports {ad_n16}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.233 [get_ports {ad_n16}]</v>
       </c>
       <c r="Y46" s="7" t="str">
         <f aca="false">CONCATENATE(IF(OR(T46="IO",T46="I"),V46,""),IF(OR(T46="IO",T46="O"),W46,""))</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.109 [get_ports {ad_n16}]
 set_input_delay -clock clk_3v3_n -max 52.062 [get_ports {ad_n16}]
 set_output_delay -clock clk_3v3_n -min -6.450 [get_ports {ad_n16}]
-set_output_delay -clock clk_3v3_n -max 53.233 [get_ports {ad_n16}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.233 [get_ports {ad_n16}]</v>
       </c>
       <c r="AG46" s="8" t="str">
         <f aca="false">IF(OR(LEFT(K46,3)="LED",LEFT(K46,16)="SBUS_DATA_OE_LED"),CONCATENATE("(",CHAR(34),"user_led",CHAR(34),", 0, Pins(",CHAR(34),D46,CHAR(34),"),  IOStandard(",CHAR(34),"lvcmos33",CHAR(34),")), ",CHAR(35),K46),"")</f>
@@ -6261,22 +6176,19 @@
       <c r="V47" s="31" t="str">
         <f aca="false">IF(AND(K47&lt;&gt;"",K47&lt;&gt;"+3v3",K47&lt;&gt;"GND",NOT(ISNA(P47)),NOT(ISNA(N47))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S47/$V$8,"0.000")," [get_ports {",K47,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S47/$W$8,"0.000")," [get_ports {",K47,"}]",CHAR(10)),"")</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.176 [get_ports {ad_n15}]
-set_input_delay -clock clk_3v3_n -max 52.151 [get_ports {ad_n15}]
-</v>
+set_input_delay -clock clk_3v3_n -max 52.151 [get_ports {ad_n15}]</v>
       </c>
       <c r="W47" s="31" t="str">
         <f aca="false">IF(AND(K47&lt;&gt;"",K47&lt;&gt;"+3v3",K47&lt;&gt;"GND",NOT(ISNA(P47)),NOT(ISNA(N47))),CONCATENATE("set_output_delay -clock clk_3v3_n -min ",TEXT(-$W$6+P47/$V$8+$P$136/$V$8,"0.000")," [get_ports {",K47,"}]",CHAR(10),"set_output_delay -clock clk_3v3_n -max ",TEXT(0.25+0.25+$W$5+P47/$W$8+$P$136/$W$8,"0.000")," [get_ports {",K47,"}]",CHAR(10)),"")</f>
         <v>set_output_delay -clock clk_3v3_n -min -6.383 [get_ports {ad_n15}]
-set_output_delay -clock clk_3v3_n -max 53.322 [get_ports {ad_n15}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.322 [get_ports {ad_n15}]</v>
       </c>
       <c r="Y47" s="7" t="str">
         <f aca="false">CONCATENATE(IF(OR(T47="IO",T47="I"),V47,""),IF(OR(T47="IO",T47="O"),W47,""))</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.176 [get_ports {ad_n15}]
 set_input_delay -clock clk_3v3_n -max 52.151 [get_ports {ad_n15}]
 set_output_delay -clock clk_3v3_n -min -6.383 [get_ports {ad_n15}]
-set_output_delay -clock clk_3v3_n -max 53.322 [get_ports {ad_n15}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.322 [get_ports {ad_n15}]</v>
       </c>
       <c r="AG47" s="8" t="str">
         <f aca="false">IF(OR(LEFT(K47,3)="LED",LEFT(K47,16)="SBUS_DATA_OE_LED"),CONCATENATE("(",CHAR(34),"user_led",CHAR(34),", 0, Pins(",CHAR(34),D47,CHAR(34),"),  IOStandard(",CHAR(34),"lvcmos33",CHAR(34),")), ",CHAR(35),K47),"")</f>
@@ -6345,22 +6257,19 @@
       <c r="V48" s="31" t="str">
         <f aca="false">IF(AND(K48&lt;&gt;"",K48&lt;&gt;"+3v3",K48&lt;&gt;"GND",NOT(ISNA(P48)),NOT(ISNA(N48))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S48/$V$8,"0.000")," [get_ports {",K48,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S48/$W$8,"0.000")," [get_ports {",K48,"}]",CHAR(10)),"")</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.121 [get_ports {ad_n14}]
-set_input_delay -clock clk_3v3_n -max 52.078 [get_ports {ad_n14}]
-</v>
+set_input_delay -clock clk_3v3_n -max 52.078 [get_ports {ad_n14}]</v>
       </c>
       <c r="W48" s="31" t="str">
         <f aca="false">IF(AND(K48&lt;&gt;"",K48&lt;&gt;"+3v3",K48&lt;&gt;"GND",NOT(ISNA(P48)),NOT(ISNA(N48))),CONCATENATE("set_output_delay -clock clk_3v3_n -min ",TEXT(-$W$6+P48/$V$8+$P$136/$V$8,"0.000")," [get_ports {",K48,"}]",CHAR(10),"set_output_delay -clock clk_3v3_n -max ",TEXT(0.25+0.25+$W$5+P48/$W$8+$P$136/$W$8,"0.000")," [get_ports {",K48,"}]",CHAR(10)),"")</f>
         <v>set_output_delay -clock clk_3v3_n -min -6.438 [get_ports {ad_n14}]
-set_output_delay -clock clk_3v3_n -max 53.249 [get_ports {ad_n14}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.249 [get_ports {ad_n14}]</v>
       </c>
       <c r="Y48" s="7" t="str">
         <f aca="false">CONCATENATE(IF(OR(T48="IO",T48="I"),V48,""),IF(OR(T48="IO",T48="O"),W48,""))</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.121 [get_ports {ad_n14}]
 set_input_delay -clock clk_3v3_n -max 52.078 [get_ports {ad_n14}]
 set_output_delay -clock clk_3v3_n -min -6.438 [get_ports {ad_n14}]
-set_output_delay -clock clk_3v3_n -max 53.249 [get_ports {ad_n14}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.249 [get_ports {ad_n14}]</v>
       </c>
       <c r="AG48" s="8" t="str">
         <f aca="false">IF(OR(LEFT(K48,3)="LED",LEFT(K48,16)="SBUS_DATA_OE_LED"),CONCATENATE("(",CHAR(34),"user_led",CHAR(34),", 0, Pins(",CHAR(34),D48,CHAR(34),"),  IOStandard(",CHAR(34),"lvcmos33",CHAR(34),")), ",CHAR(35),K48),"")</f>
@@ -6427,22 +6336,19 @@
       <c r="V49" s="31" t="str">
         <f aca="false">IF(AND(K49&lt;&gt;"",K49&lt;&gt;"+3v3",K49&lt;&gt;"GND",NOT(ISNA(P49)),NOT(ISNA(N49))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S49/$V$8,"0.000")," [get_ports {",K49,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S49/$W$8,"0.000")," [get_ports {",K49,"}]",CHAR(10)),"")</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.158 [get_ports {ad_n13}]
-set_input_delay -clock clk_3v3_n -max 52.128 [get_ports {ad_n13}]
-</v>
+set_input_delay -clock clk_3v3_n -max 52.128 [get_ports {ad_n13}]</v>
       </c>
       <c r="W49" s="31" t="str">
         <f aca="false">IF(AND(K49&lt;&gt;"",K49&lt;&gt;"+3v3",K49&lt;&gt;"GND",NOT(ISNA(P49)),NOT(ISNA(N49))),CONCATENATE("set_output_delay -clock clk_3v3_n -min ",TEXT(-$W$6+P49/$V$8+$P$136/$V$8,"0.000")," [get_ports {",K49,"}]",CHAR(10),"set_output_delay -clock clk_3v3_n -max ",TEXT(0.25+0.25+$W$5+P49/$W$8+$P$136/$W$8,"0.000")," [get_ports {",K49,"}]",CHAR(10)),"")</f>
         <v>set_output_delay -clock clk_3v3_n -min -6.401 [get_ports {ad_n13}]
-set_output_delay -clock clk_3v3_n -max 53.299 [get_ports {ad_n13}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.299 [get_ports {ad_n13}]</v>
       </c>
       <c r="Y49" s="7" t="str">
         <f aca="false">CONCATENATE(IF(OR(T49="IO",T49="I"),V49,""),IF(OR(T49="IO",T49="O"),W49,""))</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.158 [get_ports {ad_n13}]
 set_input_delay -clock clk_3v3_n -max 52.128 [get_ports {ad_n13}]
 set_output_delay -clock clk_3v3_n -min -6.401 [get_ports {ad_n13}]
-set_output_delay -clock clk_3v3_n -max 53.299 [get_ports {ad_n13}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.299 [get_ports {ad_n13}]</v>
       </c>
       <c r="AG49" s="8" t="str">
         <f aca="false">IF(OR(LEFT(K49,3)="LED",LEFT(K49,16)="SBUS_DATA_OE_LED"),CONCATENATE("(",CHAR(34),"user_led",CHAR(34),", 0, Pins(",CHAR(34),D49,CHAR(34),"),  IOStandard(",CHAR(34),"lvcmos33",CHAR(34),")), ",CHAR(35),K49),"")</f>
@@ -6509,22 +6415,19 @@
       <c r="V50" s="31" t="str">
         <f aca="false">IF(AND(K50&lt;&gt;"",K50&lt;&gt;"+3v3",K50&lt;&gt;"GND",NOT(ISNA(P50)),NOT(ISNA(N50))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S50/$V$8,"0.000")," [get_ports {",K50,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S50/$W$8,"0.000")," [get_ports {",K50,"}]",CHAR(10)),"")</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.115 [get_ports {ad_n12}]
-set_input_delay -clock clk_3v3_n -max 52.070 [get_ports {ad_n12}]
-</v>
+set_input_delay -clock clk_3v3_n -max 52.070 [get_ports {ad_n12}]</v>
       </c>
       <c r="W50" s="31" t="str">
         <f aca="false">IF(AND(K50&lt;&gt;"",K50&lt;&gt;"+3v3",K50&lt;&gt;"GND",NOT(ISNA(P50)),NOT(ISNA(N50))),CONCATENATE("set_output_delay -clock clk_3v3_n -min ",TEXT(-$W$6+P50/$V$8+$P$136/$V$8,"0.000")," [get_ports {",K50,"}]",CHAR(10),"set_output_delay -clock clk_3v3_n -max ",TEXT(0.25+0.25+$W$5+P50/$W$8+$P$136/$W$8,"0.000")," [get_ports {",K50,"}]",CHAR(10)),"")</f>
         <v>set_output_delay -clock clk_3v3_n -min -6.444 [get_ports {ad_n12}]
-set_output_delay -clock clk_3v3_n -max 53.241 [get_ports {ad_n12}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.241 [get_ports {ad_n12}]</v>
       </c>
       <c r="Y50" s="7" t="str">
         <f aca="false">CONCATENATE(IF(OR(T50="IO",T50="I"),V50,""),IF(OR(T50="IO",T50="O"),W50,""))</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.115 [get_ports {ad_n12}]
 set_input_delay -clock clk_3v3_n -max 52.070 [get_ports {ad_n12}]
 set_output_delay -clock clk_3v3_n -min -6.444 [get_ports {ad_n12}]
-set_output_delay -clock clk_3v3_n -max 53.241 [get_ports {ad_n12}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.241 [get_ports {ad_n12}]</v>
       </c>
       <c r="AG50" s="8" t="str">
         <f aca="false">IF(OR(LEFT(K50,3)="LED",LEFT(K50,16)="SBUS_DATA_OE_LED"),CONCATENATE("(",CHAR(34),"user_led",CHAR(34),", 0, Pins(",CHAR(34),D50,CHAR(34),"),  IOStandard(",CHAR(34),"lvcmos33",CHAR(34),")), ",CHAR(35),K50),"")</f>
@@ -6591,22 +6494,19 @@
       <c r="V51" s="31" t="str">
         <f aca="false">IF(AND(K51&lt;&gt;"",K51&lt;&gt;"+3v3",K51&lt;&gt;"GND",NOT(ISNA(P51)),NOT(ISNA(N51))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S51/$V$8,"0.000")," [get_ports {",K51,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S51/$W$8,"0.000")," [get_ports {",K51,"}]",CHAR(10)),"")</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.178 [get_ports {ad_n11}]
-set_input_delay -clock clk_3v3_n -max 52.155 [get_ports {ad_n11}]
-</v>
+set_input_delay -clock clk_3v3_n -max 52.155 [get_ports {ad_n11}]</v>
       </c>
       <c r="W51" s="31" t="str">
         <f aca="false">IF(AND(K51&lt;&gt;"",K51&lt;&gt;"+3v3",K51&lt;&gt;"GND",NOT(ISNA(P51)),NOT(ISNA(N51))),CONCATENATE("set_output_delay -clock clk_3v3_n -min ",TEXT(-$W$6+P51/$V$8+$P$136/$V$8,"0.000")," [get_ports {",K51,"}]",CHAR(10),"set_output_delay -clock clk_3v3_n -max ",TEXT(0.25+0.25+$W$5+P51/$W$8+$P$136/$W$8,"0.000")," [get_ports {",K51,"}]",CHAR(10)),"")</f>
         <v>set_output_delay -clock clk_3v3_n -min -6.381 [get_ports {ad_n11}]
-set_output_delay -clock clk_3v3_n -max 53.326 [get_ports {ad_n11}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.326 [get_ports {ad_n11}]</v>
       </c>
       <c r="Y51" s="7" t="str">
         <f aca="false">CONCATENATE(IF(OR(T51="IO",T51="I"),V51,""),IF(OR(T51="IO",T51="O"),W51,""))</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.178 [get_ports {ad_n11}]
 set_input_delay -clock clk_3v3_n -max 52.155 [get_ports {ad_n11}]
 set_output_delay -clock clk_3v3_n -min -6.381 [get_ports {ad_n11}]
-set_output_delay -clock clk_3v3_n -max 53.326 [get_ports {ad_n11}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.326 [get_ports {ad_n11}]</v>
       </c>
       <c r="AG51" s="8" t="str">
         <f aca="false">IF(OR(LEFT(K51,3)="LED",LEFT(K51,16)="SBUS_DATA_OE_LED"),CONCATENATE("(",CHAR(34),"user_led",CHAR(34),", 0, Pins(",CHAR(34),D51,CHAR(34),"),  IOStandard(",CHAR(34),"lvcmos33",CHAR(34),")), ",CHAR(35),K51),"")</f>
@@ -6673,22 +6573,19 @@
       <c r="V52" s="31" t="str">
         <f aca="false">IF(AND(K52&lt;&gt;"",K52&lt;&gt;"+3v3",K52&lt;&gt;"GND",NOT(ISNA(P52)),NOT(ISNA(N52))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S52/$V$8,"0.000")," [get_ports {",K52,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S52/$W$8,"0.000")," [get_ports {",K52,"}]",CHAR(10)),"")</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.129 [get_ports {ad_n10}]
-set_input_delay -clock clk_3v3_n -max 52.089 [get_ports {ad_n10}]
-</v>
+set_input_delay -clock clk_3v3_n -max 52.089 [get_ports {ad_n10}]</v>
       </c>
       <c r="W52" s="31" t="str">
         <f aca="false">IF(AND(K52&lt;&gt;"",K52&lt;&gt;"+3v3",K52&lt;&gt;"GND",NOT(ISNA(P52)),NOT(ISNA(N52))),CONCATENATE("set_output_delay -clock clk_3v3_n -min ",TEXT(-$W$6+P52/$V$8+$P$136/$V$8,"0.000")," [get_ports {",K52,"}]",CHAR(10),"set_output_delay -clock clk_3v3_n -max ",TEXT(0.25+0.25+$W$5+P52/$W$8+$P$136/$W$8,"0.000")," [get_ports {",K52,"}]",CHAR(10)),"")</f>
         <v>set_output_delay -clock clk_3v3_n -min -6.430 [get_ports {ad_n10}]
-set_output_delay -clock clk_3v3_n -max 53.260 [get_ports {ad_n10}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.260 [get_ports {ad_n10}]</v>
       </c>
       <c r="Y52" s="7" t="str">
         <f aca="false">CONCATENATE(IF(OR(T52="IO",T52="I"),V52,""),IF(OR(T52="IO",T52="O"),W52,""))</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.129 [get_ports {ad_n10}]
 set_input_delay -clock clk_3v3_n -max 52.089 [get_ports {ad_n10}]
 set_output_delay -clock clk_3v3_n -min -6.430 [get_ports {ad_n10}]
-set_output_delay -clock clk_3v3_n -max 53.260 [get_ports {ad_n10}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.260 [get_ports {ad_n10}]</v>
       </c>
       <c r="AG52" s="8" t="str">
         <f aca="false">IF(OR(LEFT(K52,3)="LED",LEFT(K52,16)="SBUS_DATA_OE_LED"),CONCATENATE("(",CHAR(34),"user_led",CHAR(34),", 0, Pins(",CHAR(34),D52,CHAR(34),"),  IOStandard(",CHAR(34),"lvcmos33",CHAR(34),")), ",CHAR(35),K52),"")</f>
@@ -6757,22 +6654,19 @@
       <c r="V53" s="31" t="str">
         <f aca="false">IF(AND(K53&lt;&gt;"",K53&lt;&gt;"+3v3",K53&lt;&gt;"GND",NOT(ISNA(P53)),NOT(ISNA(N53))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S53/$V$8,"0.000")," [get_ports {",K53,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S53/$W$8,"0.000")," [get_ports {",K53,"}]",CHAR(10)),"")</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.189 [get_ports {ad_n9}]
-set_input_delay -clock clk_3v3_n -max 52.169 [get_ports {ad_n9}]
-</v>
+set_input_delay -clock clk_3v3_n -max 52.169 [get_ports {ad_n9}]</v>
       </c>
       <c r="W53" s="31" t="str">
         <f aca="false">IF(AND(K53&lt;&gt;"",K53&lt;&gt;"+3v3",K53&lt;&gt;"GND",NOT(ISNA(P53)),NOT(ISNA(N53))),CONCATENATE("set_output_delay -clock clk_3v3_n -min ",TEXT(-$W$6+P53/$V$8+$P$136/$V$8,"0.000")," [get_ports {",K53,"}]",CHAR(10),"set_output_delay -clock clk_3v3_n -max ",TEXT(0.25+0.25+$W$5+P53/$W$8+$P$136/$W$8,"0.000")," [get_ports {",K53,"}]",CHAR(10)),"")</f>
         <v>set_output_delay -clock clk_3v3_n -min -6.370 [get_ports {ad_n9}]
-set_output_delay -clock clk_3v3_n -max 53.340 [get_ports {ad_n9}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.340 [get_ports {ad_n9}]</v>
       </c>
       <c r="Y53" s="7" t="str">
         <f aca="false">CONCATENATE(IF(OR(T53="IO",T53="I"),V53,""),IF(OR(T53="IO",T53="O"),W53,""))</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.189 [get_ports {ad_n9}]
 set_input_delay -clock clk_3v3_n -max 52.169 [get_ports {ad_n9}]
 set_output_delay -clock clk_3v3_n -min -6.370 [get_ports {ad_n9}]
-set_output_delay -clock clk_3v3_n -max 53.340 [get_ports {ad_n9}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.340 [get_ports {ad_n9}]</v>
       </c>
       <c r="AG53" s="8" t="str">
         <f aca="false">IF(OR(LEFT(K53,3)="LED",LEFT(K53,16)="SBUS_DATA_OE_LED"),CONCATENATE("(",CHAR(34),"user_led",CHAR(34),", 0, Pins(",CHAR(34),D53,CHAR(34),"),  IOStandard(",CHAR(34),"lvcmos33",CHAR(34),")), ",CHAR(35),K53),"")</f>
@@ -6839,22 +6733,19 @@
       <c r="V54" s="31" t="str">
         <f aca="false">IF(AND(K54&lt;&gt;"",K54&lt;&gt;"+3v3",K54&lt;&gt;"GND",NOT(ISNA(P54)),NOT(ISNA(N54))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S54/$V$8,"0.000")," [get_ports {",K54,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S54/$W$8,"0.000")," [get_ports {",K54,"}]",CHAR(10)),"")</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.139 [get_ports {ad_n8}]
-set_input_delay -clock clk_3v3_n -max 52.102 [get_ports {ad_n8}]
-</v>
+set_input_delay -clock clk_3v3_n -max 52.102 [get_ports {ad_n8}]</v>
       </c>
       <c r="W54" s="31" t="str">
         <f aca="false">IF(AND(K54&lt;&gt;"",K54&lt;&gt;"+3v3",K54&lt;&gt;"GND",NOT(ISNA(P54)),NOT(ISNA(N54))),CONCATENATE("set_output_delay -clock clk_3v3_n -min ",TEXT(-$W$6+P54/$V$8+$P$136/$V$8,"0.000")," [get_ports {",K54,"}]",CHAR(10),"set_output_delay -clock clk_3v3_n -max ",TEXT(0.25+0.25+$W$5+P54/$W$8+$P$136/$W$8,"0.000")," [get_ports {",K54,"}]",CHAR(10)),"")</f>
         <v>set_output_delay -clock clk_3v3_n -min -6.420 [get_ports {ad_n8}]
-set_output_delay -clock clk_3v3_n -max 53.273 [get_ports {ad_n8}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.273 [get_ports {ad_n8}]</v>
       </c>
       <c r="Y54" s="7" t="str">
         <f aca="false">CONCATENATE(IF(OR(T54="IO",T54="I"),V54,""),IF(OR(T54="IO",T54="O"),W54,""))</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.139 [get_ports {ad_n8}]
 set_input_delay -clock clk_3v3_n -max 52.102 [get_ports {ad_n8}]
 set_output_delay -clock clk_3v3_n -min -6.420 [get_ports {ad_n8}]
-set_output_delay -clock clk_3v3_n -max 53.273 [get_ports {ad_n8}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.273 [get_ports {ad_n8}]</v>
       </c>
       <c r="AG54" s="8" t="str">
         <f aca="false">IF(OR(LEFT(K54,3)="LED",LEFT(K54,16)="SBUS_DATA_OE_LED"),CONCATENATE("(",CHAR(34),"user_led",CHAR(34),", 0, Pins(",CHAR(34),D54,CHAR(34),"),  IOStandard(",CHAR(34),"lvcmos33",CHAR(34),")), ",CHAR(35),K54),"")</f>
@@ -6921,22 +6812,19 @@
       <c r="V55" s="31" t="str">
         <f aca="false">IF(AND(K55&lt;&gt;"",K55&lt;&gt;"+3v3",K55&lt;&gt;"GND",NOT(ISNA(P55)),NOT(ISNA(N55))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S55/$V$8,"0.000")," [get_ports {",K55,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S55/$W$8,"0.000")," [get_ports {",K55,"}]",CHAR(10)),"")</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.168 [get_ports {ad_n7}]
-set_input_delay -clock clk_3v3_n -max 52.141 [get_ports {ad_n7}]
-</v>
+set_input_delay -clock clk_3v3_n -max 52.141 [get_ports {ad_n7}]</v>
       </c>
       <c r="W55" s="31" t="str">
         <f aca="false">IF(AND(K55&lt;&gt;"",K55&lt;&gt;"+3v3",K55&lt;&gt;"GND",NOT(ISNA(P55)),NOT(ISNA(N55))),CONCATENATE("set_output_delay -clock clk_3v3_n -min ",TEXT(-$W$6+P55/$V$8+$P$136/$V$8,"0.000")," [get_ports {",K55,"}]",CHAR(10),"set_output_delay -clock clk_3v3_n -max ",TEXT(0.25+0.25+$W$5+P55/$W$8+$P$136/$W$8,"0.000")," [get_ports {",K55,"}]",CHAR(10)),"")</f>
         <v>set_output_delay -clock clk_3v3_n -min -6.391 [get_ports {ad_n7}]
-set_output_delay -clock clk_3v3_n -max 53.312 [get_ports {ad_n7}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.312 [get_ports {ad_n7}]</v>
       </c>
       <c r="Y55" s="7" t="str">
         <f aca="false">CONCATENATE(IF(OR(T55="IO",T55="I"),V55,""),IF(OR(T55="IO",T55="O"),W55,""))</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.168 [get_ports {ad_n7}]
 set_input_delay -clock clk_3v3_n -max 52.141 [get_ports {ad_n7}]
 set_output_delay -clock clk_3v3_n -min -6.391 [get_ports {ad_n7}]
-set_output_delay -clock clk_3v3_n -max 53.312 [get_ports {ad_n7}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.312 [get_ports {ad_n7}]</v>
       </c>
       <c r="AG55" s="8" t="str">
         <f aca="false">IF(OR(LEFT(K55,3)="LED",LEFT(K55,16)="SBUS_DATA_OE_LED"),CONCATENATE("(",CHAR(34),"user_led",CHAR(34),", 0, Pins(",CHAR(34),D55,CHAR(34),"),  IOStandard(",CHAR(34),"lvcmos33",CHAR(34),")), ",CHAR(35),K55),"")</f>
@@ -7003,22 +6891,19 @@
       <c r="V56" s="31" t="str">
         <f aca="false">IF(AND(K56&lt;&gt;"",K56&lt;&gt;"+3v3",K56&lt;&gt;"GND",NOT(ISNA(P56)),NOT(ISNA(N56))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S56/$V$8,"0.000")," [get_ports {",K56,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S56/$W$8,"0.000")," [get_ports {",K56,"}]",CHAR(10)),"")</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.136 [get_ports {ad_n6}]
-set_input_delay -clock clk_3v3_n -max 52.097 [get_ports {ad_n6}]
-</v>
+set_input_delay -clock clk_3v3_n -max 52.097 [get_ports {ad_n6}]</v>
       </c>
       <c r="W56" s="31" t="str">
         <f aca="false">IF(AND(K56&lt;&gt;"",K56&lt;&gt;"+3v3",K56&lt;&gt;"GND",NOT(ISNA(P56)),NOT(ISNA(N56))),CONCATENATE("set_output_delay -clock clk_3v3_n -min ",TEXT(-$W$6+P56/$V$8+$P$136/$V$8,"0.000")," [get_ports {",K56,"}]",CHAR(10),"set_output_delay -clock clk_3v3_n -max ",TEXT(0.25+0.25+$W$5+P56/$W$8+$P$136/$W$8,"0.000")," [get_ports {",K56,"}]",CHAR(10)),"")</f>
         <v>set_output_delay -clock clk_3v3_n -min -6.423 [get_ports {ad_n6}]
-set_output_delay -clock clk_3v3_n -max 53.269 [get_ports {ad_n6}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.269 [get_ports {ad_n6}]</v>
       </c>
       <c r="Y56" s="7" t="str">
         <f aca="false">CONCATENATE(IF(OR(T56="IO",T56="I"),V56,""),IF(OR(T56="IO",T56="O"),W56,""))</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.136 [get_ports {ad_n6}]
 set_input_delay -clock clk_3v3_n -max 52.097 [get_ports {ad_n6}]
 set_output_delay -clock clk_3v3_n -min -6.423 [get_ports {ad_n6}]
-set_output_delay -clock clk_3v3_n -max 53.269 [get_ports {ad_n6}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.269 [get_ports {ad_n6}]</v>
       </c>
       <c r="AG56" s="8" t="str">
         <f aca="false">IF(OR(LEFT(K56,3)="LED",LEFT(K56,16)="SBUS_DATA_OE_LED"),CONCATENATE("(",CHAR(34),"user_led",CHAR(34),", 0, Pins(",CHAR(34),D56,CHAR(34),"),  IOStandard(",CHAR(34),"lvcmos33",CHAR(34),")), ",CHAR(35),K56),"")</f>
@@ -7085,22 +6970,19 @@
       <c r="V57" s="31" t="str">
         <f aca="false">IF(AND(K57&lt;&gt;"",K57&lt;&gt;"+3v3",K57&lt;&gt;"GND",NOT(ISNA(P57)),NOT(ISNA(N57))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S57/$V$8,"0.000")," [get_ports {",K57,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S57/$W$8,"0.000")," [get_ports {",K57,"}]",CHAR(10)),"")</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.181 [get_ports {ad_n5}]
-set_input_delay -clock clk_3v3_n -max 52.158 [get_ports {ad_n5}]
-</v>
+set_input_delay -clock clk_3v3_n -max 52.158 [get_ports {ad_n5}]</v>
       </c>
       <c r="W57" s="31" t="str">
         <f aca="false">IF(AND(K57&lt;&gt;"",K57&lt;&gt;"+3v3",K57&lt;&gt;"GND",NOT(ISNA(P57)),NOT(ISNA(N57))),CONCATENATE("set_output_delay -clock clk_3v3_n -min ",TEXT(-$W$6+P57/$V$8+$P$136/$V$8,"0.000")," [get_ports {",K57,"}]",CHAR(10),"set_output_delay -clock clk_3v3_n -max ",TEXT(0.25+0.25+$W$5+P57/$W$8+$P$136/$W$8,"0.000")," [get_ports {",K57,"}]",CHAR(10)),"")</f>
         <v>set_output_delay -clock clk_3v3_n -min -6.378 [get_ports {ad_n5}]
-set_output_delay -clock clk_3v3_n -max 53.329 [get_ports {ad_n5}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.329 [get_ports {ad_n5}]</v>
       </c>
       <c r="Y57" s="7" t="str">
         <f aca="false">CONCATENATE(IF(OR(T57="IO",T57="I"),V57,""),IF(OR(T57="IO",T57="O"),W57,""))</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.181 [get_ports {ad_n5}]
 set_input_delay -clock clk_3v3_n -max 52.158 [get_ports {ad_n5}]
 set_output_delay -clock clk_3v3_n -min -6.378 [get_ports {ad_n5}]
-set_output_delay -clock clk_3v3_n -max 53.329 [get_ports {ad_n5}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.329 [get_ports {ad_n5}]</v>
       </c>
       <c r="AG57" s="8" t="str">
         <f aca="false">IF(OR(LEFT(K57,3)="LED",LEFT(K57,16)="SBUS_DATA_OE_LED"),CONCATENATE("(",CHAR(34),"user_led",CHAR(34),", 0, Pins(",CHAR(34),D57,CHAR(34),"),  IOStandard(",CHAR(34),"lvcmos33",CHAR(34),")), ",CHAR(35),K57),"")</f>
@@ -7167,22 +7049,19 @@
       <c r="V58" s="31" t="str">
         <f aca="false">IF(AND(K58&lt;&gt;"",K58&lt;&gt;"+3v3",K58&lt;&gt;"GND",NOT(ISNA(P58)),NOT(ISNA(N58))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S58/$V$8,"0.000")," [get_ports {",K58,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S58/$W$8,"0.000")," [get_ports {",K58,"}]",CHAR(10)),"")</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.156 [get_ports {ad_n4}]
-set_input_delay -clock clk_3v3_n -max 52.124 [get_ports {ad_n4}]
-</v>
+set_input_delay -clock clk_3v3_n -max 52.124 [get_ports {ad_n4}]</v>
       </c>
       <c r="W58" s="31" t="str">
         <f aca="false">IF(AND(K58&lt;&gt;"",K58&lt;&gt;"+3v3",K58&lt;&gt;"GND",NOT(ISNA(P58)),NOT(ISNA(N58))),CONCATENATE("set_output_delay -clock clk_3v3_n -min ",TEXT(-$W$6+P58/$V$8+$P$136/$V$8,"0.000")," [get_ports {",K58,"}]",CHAR(10),"set_output_delay -clock clk_3v3_n -max ",TEXT(0.25+0.25+$W$5+P58/$W$8+$P$136/$W$8,"0.000")," [get_ports {",K58,"}]",CHAR(10)),"")</f>
         <v>set_output_delay -clock clk_3v3_n -min -6.403 [get_ports {ad_n4}]
-set_output_delay -clock clk_3v3_n -max 53.295 [get_ports {ad_n4}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.295 [get_ports {ad_n4}]</v>
       </c>
       <c r="Y58" s="7" t="str">
         <f aca="false">CONCATENATE(IF(OR(T58="IO",T58="I"),V58,""),IF(OR(T58="IO",T58="O"),W58,""))</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.156 [get_ports {ad_n4}]
 set_input_delay -clock clk_3v3_n -max 52.124 [get_ports {ad_n4}]
 set_output_delay -clock clk_3v3_n -min -6.403 [get_ports {ad_n4}]
-set_output_delay -clock clk_3v3_n -max 53.295 [get_ports {ad_n4}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.295 [get_ports {ad_n4}]</v>
       </c>
       <c r="AG58" s="8" t="str">
         <f aca="false">IF(OR(LEFT(K58,3)="LED",LEFT(K58,16)="SBUS_DATA_OE_LED"),CONCATENATE("(",CHAR(34),"user_led",CHAR(34),", 0, Pins(",CHAR(34),D58,CHAR(34),"),  IOStandard(",CHAR(34),"lvcmos33",CHAR(34),")), ",CHAR(35),K58),"")</f>
@@ -7249,22 +7128,19 @@
       <c r="V59" s="31" t="str">
         <f aca="false">IF(AND(K59&lt;&gt;"",K59&lt;&gt;"+3v3",K59&lt;&gt;"GND",NOT(ISNA(P59)),NOT(ISNA(N59))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S59/$V$8,"0.000")," [get_ports {",K59,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S59/$W$8,"0.000")," [get_ports {",K59,"}]",CHAR(10)),"")</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.209 [get_ports {ad_n3}]
-set_input_delay -clock clk_3v3_n -max 52.195 [get_ports {ad_n3}]
-</v>
+set_input_delay -clock clk_3v3_n -max 52.195 [get_ports {ad_n3}]</v>
       </c>
       <c r="W59" s="31" t="str">
         <f aca="false">IF(AND(K59&lt;&gt;"",K59&lt;&gt;"+3v3",K59&lt;&gt;"GND",NOT(ISNA(P59)),NOT(ISNA(N59))),CONCATENATE("set_output_delay -clock clk_3v3_n -min ",TEXT(-$W$6+P59/$V$8+$P$136/$V$8,"0.000")," [get_ports {",K59,"}]",CHAR(10),"set_output_delay -clock clk_3v3_n -max ",TEXT(0.25+0.25+$W$5+P59/$W$8+$P$136/$W$8,"0.000")," [get_ports {",K59,"}]",CHAR(10)),"")</f>
         <v>set_output_delay -clock clk_3v3_n -min -6.350 [get_ports {ad_n3}]
-set_output_delay -clock clk_3v3_n -max 53.366 [get_ports {ad_n3}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.366 [get_ports {ad_n3}]</v>
       </c>
       <c r="Y59" s="7" t="str">
         <f aca="false">CONCATENATE(IF(OR(T59="IO",T59="I"),V59,""),IF(OR(T59="IO",T59="O"),W59,""))</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.209 [get_ports {ad_n3}]
 set_input_delay -clock clk_3v3_n -max 52.195 [get_ports {ad_n3}]
 set_output_delay -clock clk_3v3_n -min -6.350 [get_ports {ad_n3}]
-set_output_delay -clock clk_3v3_n -max 53.366 [get_ports {ad_n3}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.366 [get_ports {ad_n3}]</v>
       </c>
       <c r="AG59" s="8" t="str">
         <f aca="false">IF(OR(LEFT(K59,3)="LED",LEFT(K59,16)="SBUS_DATA_OE_LED"),CONCATENATE("(",CHAR(34),"user_led",CHAR(34),", 0, Pins(",CHAR(34),D59,CHAR(34),"),  IOStandard(",CHAR(34),"lvcmos33",CHAR(34),")), ",CHAR(35),K59),"")</f>
@@ -7495,22 +7371,19 @@
       <c r="V62" s="31" t="str">
         <f aca="false">IF(AND(K62&lt;&gt;"",K62&lt;&gt;"+3v3",K62&lt;&gt;"GND",NOT(ISNA(P62)),NOT(ISNA(N62))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S62/$V$8,"0.000")," [get_ports {",K62,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S62/$W$8,"0.000")," [get_ports {",K62,"}]",CHAR(10)),"")</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.257 [get_ports {ad_n0}]
-set_input_delay -clock clk_3v3_n -max 52.259 [get_ports {ad_n0}]
-</v>
+set_input_delay -clock clk_3v3_n -max 52.259 [get_ports {ad_n0}]</v>
       </c>
       <c r="W62" s="31" t="str">
         <f aca="false">IF(AND(K62&lt;&gt;"",K62&lt;&gt;"+3v3",K62&lt;&gt;"GND",NOT(ISNA(P62)),NOT(ISNA(N62))),CONCATENATE("set_output_delay -clock clk_3v3_n -min ",TEXT(-$W$6+P62/$V$8+$P$136/$V$8,"0.000")," [get_ports {",K62,"}]",CHAR(10),"set_output_delay -clock clk_3v3_n -max ",TEXT(0.25+0.25+$W$5+P62/$W$8+$P$136/$W$8,"0.000")," [get_ports {",K62,"}]",CHAR(10)),"")</f>
         <v>set_output_delay -clock clk_3v3_n -min -6.302 [get_ports {ad_n0}]
-set_output_delay -clock clk_3v3_n -max 53.430 [get_ports {ad_n0}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.430 [get_ports {ad_n0}]</v>
       </c>
       <c r="Y62" s="7" t="str">
         <f aca="false">CONCATENATE(IF(OR(T62="IO",T62="I"),V62,""),IF(OR(T62="IO",T62="O"),W62,""))</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.257 [get_ports {ad_n0}]
 set_input_delay -clock clk_3v3_n -max 52.259 [get_ports {ad_n0}]
 set_output_delay -clock clk_3v3_n -min -6.302 [get_ports {ad_n0}]
-set_output_delay -clock clk_3v3_n -max 53.430 [get_ports {ad_n0}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.430 [get_ports {ad_n0}]</v>
       </c>
       <c r="AG62" s="8" t="str">
         <f aca="false">IF(OR(LEFT(K62,3)="LED",LEFT(K62,16)="SBUS_DATA_OE_LED"),CONCATENATE("(",CHAR(34),"user_led",CHAR(34),", 0, Pins(",CHAR(34),D62,CHAR(34),"),  IOStandard(",CHAR(34),"lvcmos33",CHAR(34),")), ",CHAR(35),K62),"")</f>
@@ -8643,8 +8516,7 @@
       <c r="U79" s="30" t="str">
         <f aca="false">IF(AND(K79&lt;&gt;"",K79&lt;&gt;"+3v3",K79&lt;&gt;"GND"),CONCATENATE("set_property PACKAGE_PIN ",D79," [get_ports {",K79,"}]",CHAR(10),"set_property IOSTANDARD LVTTL [get_ports {",K79,"}]",CHAR(10)),"")</f>
         <v>set_property PACKAGE_PIN U6 [get_ports {arb_n3}]
-set_property IOSTANDARD LVTTL [get_ports {arb_n3}]
-</v>
+set_property IOSTANDARD LVTTL [get_ports {arb_n3}]</v>
       </c>
       <c r="V79" s="31" t="str">
         <f aca="false">IF(AND(K79&lt;&gt;"",K79&lt;&gt;"+3v3",K79&lt;&gt;"GND",NOT(ISNA(P79)),NOT(ISNA(N79))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S79/$V$8,"0.000")," [get_ports {",K79,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S79/$W$8,"0.000")," [get_ports {",K79,"}]",CHAR(10)),"")</f>
@@ -8715,8 +8587,7 @@
       <c r="U80" s="30" t="str">
         <f aca="false">IF(AND(K80&lt;&gt;"",K80&lt;&gt;"+3v3",K80&lt;&gt;"GND"),CONCATENATE("set_property PACKAGE_PIN ",D80," [get_ports {",K80,"}]",CHAR(10),"set_property IOSTANDARD LVTTL [get_ports {",K80,"}]",CHAR(10)),"")</f>
         <v>set_property PACKAGE_PIN V5 [get_ports {arb_n2}]
-set_property IOSTANDARD LVTTL [get_ports {arb_n2}]
-</v>
+set_property IOSTANDARD LVTTL [get_ports {arb_n2}]</v>
       </c>
       <c r="V80" s="31" t="str">
         <f aca="false">IF(AND(K80&lt;&gt;"",K80&lt;&gt;"+3v3",K80&lt;&gt;"GND",NOT(ISNA(P80)),NOT(ISNA(N80))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S80/$V$8,"0.000")," [get_ports {",K80,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S80/$W$8,"0.000")," [get_ports {",K80,"}]",CHAR(10)),"")</f>
@@ -8787,8 +8658,7 @@
       <c r="U81" s="30" t="str">
         <f aca="false">IF(AND(K81&lt;&gt;"",K81&lt;&gt;"+3v3",K81&lt;&gt;"GND"),CONCATENATE("set_property PACKAGE_PIN ",D81," [get_ports {",K81,"}]",CHAR(10),"set_property IOSTANDARD LVTTL [get_ports {",K81,"}]",CHAR(10)),"")</f>
         <v>set_property PACKAGE_PIN T8 [get_ports {arb_n0}]
-set_property IOSTANDARD LVTTL [get_ports {arb_n0}]
-</v>
+set_property IOSTANDARD LVTTL [get_ports {arb_n0}]</v>
       </c>
       <c r="V81" s="31" t="str">
         <f aca="false">IF(AND(K81&lt;&gt;"",K81&lt;&gt;"+3v3",K81&lt;&gt;"GND",NOT(ISNA(P81)),NOT(ISNA(N81))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S81/$V$8,"0.000")," [get_ports {",K81,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S81/$W$8,"0.000")," [get_ports {",K81,"}]",CHAR(10)),"")</f>
@@ -8863,8 +8733,7 @@
       <c r="U82" s="30" t="str">
         <f aca="false">IF(AND(K82&lt;&gt;"",K82&lt;&gt;"+3v3",K82&lt;&gt;"GND"),CONCATENATE("set_property PACKAGE_PIN ",D82," [get_ports {",K82,"}]",CHAR(10),"set_property IOSTANDARD LVTTL [get_ports {",K82,"}]",CHAR(10)),"")</f>
         <v>set_property PACKAGE_PIN V4 [get_ports {arb_n1}]
-set_property IOSTANDARD LVTTL [get_ports {arb_n1}]
-</v>
+set_property IOSTANDARD LVTTL [get_ports {arb_n1}]</v>
       </c>
       <c r="V82" s="31" t="str">
         <f aca="false">IF(AND(K82&lt;&gt;"",K82&lt;&gt;"+3v3",K82&lt;&gt;"GND",NOT(ISNA(P82)),NOT(ISNA(N82))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S82/$V$8,"0.000")," [get_ports {",K82,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S82/$W$8,"0.000")," [get_ports {",K82,"}]",CHAR(10)),"")</f>
@@ -8935,8 +8804,7 @@
       <c r="U83" s="30" t="str">
         <f aca="false">IF(AND(K83&lt;&gt;"",K83&lt;&gt;"+3v3",K83&lt;&gt;"GND"),CONCATENATE("set_property PACKAGE_PIN ",D83," [get_ports {",K83,"}]",CHAR(10),"set_property IOSTANDARD LVTTL [get_ports {",K83,"}]",CHAR(10)),"")</f>
         <v>set_property PACKAGE_PIN R8 [get_ports {tmx_oe_n}]
-set_property IOSTANDARD LVTTL [get_ports {tmx_oe_n}]
-</v>
+set_property IOSTANDARD LVTTL [get_ports {tmx_oe_n}]</v>
       </c>
       <c r="V83" s="31" t="str">
         <f aca="false">IF(AND(K83&lt;&gt;"",K83&lt;&gt;"+3v3",K83&lt;&gt;"GND",NOT(ISNA(P83)),NOT(ISNA(N83))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S83/$V$8,"0.000")," [get_ports {",K83,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S83/$W$8,"0.000")," [get_ports {",K83,"}]",CHAR(10)),"")</f>
@@ -9009,20 +8877,17 @@
       <c r="U84" s="30" t="str">
         <f aca="false">IF(AND(K84&lt;&gt;"",K84&lt;&gt;"+3v3",K84&lt;&gt;"GND"),CONCATENATE("set_property PACKAGE_PIN ",D84," [get_ports {",K84,"}]",CHAR(10),"set_property IOSTANDARD LVTTL [get_ports {",K84,"}]",CHAR(10)),"")</f>
         <v>set_property PACKAGE_PIN T5 [get_ports {clk2x_n}]
-set_property IOSTANDARD LVTTL [get_ports {clk2x_n}]
-</v>
+set_property IOSTANDARD LVTTL [get_ports {clk2x_n}]</v>
       </c>
       <c r="V84" s="31" t="str">
         <f aca="false">IF(AND(K84&lt;&gt;"",K84&lt;&gt;"+3v3",K84&lt;&gt;"GND",NOT(ISNA(P84)),NOT(ISNA(N84))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S84/$V$8,"0.000")," [get_ports {",K84,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S84/$W$8,"0.000")," [get_ports {",K84,"}]",CHAR(10)),"")</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.495 [get_ports {clk2x_n}]
-set_input_delay -clock clk_3v3_n -max 52.576 [get_ports {clk2x_n}]
-</v>
+set_input_delay -clock clk_3v3_n -max 52.576 [get_ports {clk2x_n}]</v>
       </c>
       <c r="W84" s="31" t="str">
         <f aca="false">IF(AND(K84&lt;&gt;"",K84&lt;&gt;"+3v3",K84&lt;&gt;"GND",NOT(ISNA(P84)),NOT(ISNA(N84))),CONCATENATE("set_output_delay -clock clk_3v3_n -min ",TEXT(-$W$6+P84/$V$8+$P$136/$V$8,"0.000")," [get_ports {",K84,"}]",CHAR(10),"set_output_delay -clock clk_3v3_n -max ",TEXT(0.25+0.25+$W$5+P84/$W$8+$P$136/$W$8,"0.000")," [get_ports {",K84,"}]",CHAR(10)),"")</f>
         <v>set_output_delay -clock clk_3v3_n -min -6.064 [get_ports {clk2x_n}]
-set_output_delay -clock clk_3v3_n -max 53.747 [get_ports {clk2x_n}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.747 [get_ports {clk2x_n}]</v>
       </c>
       <c r="Y84" s="7" t="str">
         <f aca="false">CONCATENATE(IF(OR(T84="IO",T84="I"),V84,""),IF(OR(T84="IO",T84="O"),W84,""))</f>
@@ -9085,8 +8950,7 @@
       <c r="U85" s="30" t="str">
         <f aca="false">IF(AND(K85&lt;&gt;"",K85&lt;&gt;"+3v3",K85&lt;&gt;"GND"),CONCATENATE("set_property PACKAGE_PIN ",D85," [get_ports {",K85,"}]",CHAR(10),"set_property IOSTANDARD LVTTL [get_ports {",K85,"}]",CHAR(10)),"")</f>
         <v>set_property PACKAGE_PIN R7 [get_ports {tm_n_o1}]
-set_property IOSTANDARD LVTTL [get_ports {tm_n_o1}]
-</v>
+set_property IOSTANDARD LVTTL [get_ports {tm_n_o1}]</v>
       </c>
       <c r="V85" s="31" t="str">
         <f aca="false">IF(AND(K85&lt;&gt;"",K85&lt;&gt;"+3v3",K85&lt;&gt;"GND",NOT(ISNA(P85)),NOT(ISNA(N85))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S85/$V$8,"0.000")," [get_ports {",K85,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S85/$W$8,"0.000")," [get_ports {",K85,"}]",CHAR(10)),"")</f>
@@ -9137,7 +9001,7 @@
       </c>
       <c r="K86" s="3" t="str">
         <f aca="false">IF(NOT(ISNA($H86)),$H86,"")</f>
-        <v>SD_D1</v>
+        <v>SD_D2</v>
       </c>
       <c r="M86" s="0" t="n">
         <f aca="false">VLOOKUP(A86,'2.13 ping -&gt; trace length'!$A$1:$B$103,2,0)</f>
@@ -9164,9 +9028,8 @@
       </c>
       <c r="U86" s="30" t="str">
         <f aca="false">IF(AND(K86&lt;&gt;"",K86&lt;&gt;"+3v3",K86&lt;&gt;"GND"),CONCATENATE("set_property PACKAGE_PIN ",D86," [get_ports {",K86,"}]",CHAR(10),"set_property IOSTANDARD LVTTL [get_ports {",K86,"}]",CHAR(10)),"")</f>
-        <v>set_property PACKAGE_PIN T4 [get_ports {SD_D1}]
-set_property IOSTANDARD LVTTL [get_ports {SD_D1}]
-</v>
+        <v>set_property PACKAGE_PIN T4 [get_ports {SD_D2}]
+set_property IOSTANDARD LVTTL [get_ports {SD_D2}]</v>
       </c>
       <c r="V86" s="31" t="str">
         <f aca="false">IF(AND(K86&lt;&gt;"",K86&lt;&gt;"+3v3",K86&lt;&gt;"GND",NOT(ISNA(P86)),NOT(ISNA(N86))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S86/$V$8,"0.000")," [get_ports {",K86,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S86/$W$8,"0.000")," [get_ports {",K86,"}]",CHAR(10)),"")</f>
@@ -9237,8 +9100,7 @@
       <c r="U87" s="30" t="str">
         <f aca="false">IF(AND(K87&lt;&gt;"",K87&lt;&gt;"+3v3",K87&lt;&gt;"GND"),CONCATENATE("set_property PACKAGE_PIN ",D87," [get_ports {",K87,"}]",CHAR(10),"set_property IOSTANDARD LVTTL [get_ports {",K87,"}]",CHAR(10)),"")</f>
         <v>set_property PACKAGE_PIN T6 [get_ports {tm_n_o0}]
-set_property IOSTANDARD LVTTL [get_ports {tm_n_o0}]
-</v>
+set_property IOSTANDARD LVTTL [get_ports {tm_n_o0}]</v>
       </c>
       <c r="V87" s="31" t="str">
         <f aca="false">IF(AND(K87&lt;&gt;"",K87&lt;&gt;"+3v3",K87&lt;&gt;"GND",NOT(ISNA(P87)),NOT(ISNA(N87))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S87/$V$8,"0.000")," [get_ports {",K87,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S87/$W$8,"0.000")," [get_ports {",K87,"}]",CHAR(10)),"")</f>
@@ -9284,7 +9146,7 @@
       </c>
       <c r="K88" s="3" t="str">
         <f aca="false">IF(NOT(ISNA($H88)),$H88,"")</f>
-        <v>SD_D0</v>
+        <v>SD_D3</v>
       </c>
       <c r="M88" s="0" t="n">
         <f aca="false">VLOOKUP(A88,'2.13 ping -&gt; trace length'!$A$1:$B$103,2,0)</f>
@@ -9308,9 +9170,8 @@
       </c>
       <c r="U88" s="30" t="str">
         <f aca="false">IF(AND(K88&lt;&gt;"",K88&lt;&gt;"+3v3",K88&lt;&gt;"GND"),CONCATENATE("set_property PACKAGE_PIN ",D88," [get_ports {",K88,"}]",CHAR(10),"set_property IOSTANDARD LVTTL [get_ports {",K88,"}]",CHAR(10)),"")</f>
-        <v>set_property PACKAGE_PIN U4 [get_ports {SD_D0}]
-set_property IOSTANDARD LVTTL [get_ports {SD_D0}]
-</v>
+        <v>set_property PACKAGE_PIN U4 [get_ports {SD_D3}]
+set_property IOSTANDARD LVTTL [get_ports {SD_D3}]</v>
       </c>
       <c r="V88" s="31" t="str">
         <f aca="false">IF(AND(K88&lt;&gt;"",K88&lt;&gt;"+3v3",K88&lt;&gt;"GND",NOT(ISNA(P88)),NOT(ISNA(N88))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S88/$V$8,"0.000")," [get_ports {",K88,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S88/$W$8,"0.000")," [get_ports {",K88,"}]",CHAR(10)),"")</f>
@@ -9443,7 +9304,7 @@
       </c>
       <c r="K90" s="3" t="str">
         <f aca="false">IF(NOT(ISNA($H90)),$H90,"")</f>
-        <v>SD_CLK</v>
+        <v>SD_CMD</v>
       </c>
       <c r="M90" s="0" t="n">
         <f aca="false">VLOOKUP(A90,'2.13 ping -&gt; trace length'!$A$1:$B$103,2,0)</f>
@@ -9467,9 +9328,8 @@
       </c>
       <c r="U90" s="30" t="str">
         <f aca="false">IF(AND(K90&lt;&gt;"",K90&lt;&gt;"+3v3",K90&lt;&gt;"GND"),CONCATENATE("set_property PACKAGE_PIN ",D90," [get_ports {",K90,"}]",CHAR(10),"set_property IOSTANDARD LVTTL [get_ports {",K90,"}]",CHAR(10)),"")</f>
-        <v>set_property PACKAGE_PIN U3 [get_ports {SD_CLK}]
-set_property IOSTANDARD LVTTL [get_ports {SD_CLK}]
-</v>
+        <v>set_property PACKAGE_PIN U3 [get_ports {SD_CMD}]
+set_property IOSTANDARD LVTTL [get_ports {SD_CMD}]</v>
       </c>
       <c r="V90" s="31" t="str">
         <f aca="false">IF(AND(K90&lt;&gt;"",K90&lt;&gt;"+3v3",K90&lt;&gt;"GND",NOT(ISNA(P90)),NOT(ISNA(N90))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S90/$V$8,"0.000")," [get_ports {",K90,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S90/$W$8,"0.000")," [get_ports {",K90,"}]",CHAR(10)),"")</f>
@@ -9604,7 +9464,7 @@
       </c>
       <c r="K92" s="3" t="str">
         <f aca="false">IF(NOT(ISNA($H92)),$H92,"")</f>
-        <v>SD_CMD</v>
+        <v>SD_CLK</v>
       </c>
       <c r="M92" s="0" t="n">
         <f aca="false">VLOOKUP(A92,'2.13 ping -&gt; trace length'!$A$1:$B$103,2,0)</f>
@@ -9628,9 +9488,8 @@
       </c>
       <c r="U92" s="30" t="str">
         <f aca="false">IF(AND(K92&lt;&gt;"",K92&lt;&gt;"+3v3",K92&lt;&gt;"GND"),CONCATENATE("set_property PACKAGE_PIN ",D92," [get_ports {",K92,"}]",CHAR(10),"set_property IOSTANDARD LVTTL [get_ports {",K92,"}]",CHAR(10)),"")</f>
-        <v>set_property PACKAGE_PIN V1 [get_ports {SD_CMD}]
-set_property IOSTANDARD LVTTL [get_ports {SD_CMD}]
-</v>
+        <v>set_property PACKAGE_PIN V1 [get_ports {SD_CLK}]
+set_property IOSTANDARD LVTTL [get_ports {SD_CLK}]</v>
       </c>
       <c r="V92" s="31" t="str">
         <f aca="false">IF(AND(K92&lt;&gt;"",K92&lt;&gt;"+3v3",K92&lt;&gt;"GND",NOT(ISNA(P92)),NOT(ISNA(N92))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S92/$V$8,"0.000")," [get_ports {",K92,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S92/$W$8,"0.000")," [get_ports {",K92,"}]",CHAR(10)),"")</f>
@@ -9657,7 +9516,7 @@
       </c>
       <c r="AE92" s="0" t="str">
         <f aca="false">H92</f>
-        <v>SD_CMD</v>
+        <v>SD_CLK</v>
       </c>
       <c r="AG92" s="8" t="str">
         <f aca="false">IF(OR(LEFT(K92,3)="LED",LEFT(K92,16)="SBUS_DATA_OE_LED"),CONCATENATE("(",CHAR(34),"user_led",CHAR(34),", 0, Pins(",CHAR(34),D92,CHAR(34),"),  IOStandard(",CHAR(34),"lvcmos33",CHAR(34),")), ",CHAR(35),K92),"")</f>
@@ -9691,7 +9550,7 @@
       </c>
       <c r="K93" s="3" t="str">
         <f aca="false">IF(NOT(ISNA($H93)),$H93,"")</f>
-        <v>tm_n0</v>
+        <v>tm_n1</v>
       </c>
       <c r="M93" s="0" t="n">
         <f aca="false">VLOOKUP(A93,'2.13 ping -&gt; trace length'!$A$1:$B$103,2,0)</f>
@@ -9715,9 +9574,8 @@
       </c>
       <c r="U93" s="30" t="str">
         <f aca="false">IF(AND(K93&lt;&gt;"",K93&lt;&gt;"+3v3",K93&lt;&gt;"GND"),CONCATENATE("set_property PACKAGE_PIN ",D93," [get_ports {",K93,"}]",CHAR(10),"set_property IOSTANDARD LVTTL [get_ports {",K93,"}]",CHAR(10)),"")</f>
-        <v>set_property PACKAGE_PIN V2 [get_ports {tm_n0}]
-set_property IOSTANDARD LVTTL [get_ports {tm_n0}]
-</v>
+        <v>set_property PACKAGE_PIN V2 [get_ports {tm_n1}]
+set_property IOSTANDARD LVTTL [get_ports {tm_n1}]</v>
       </c>
       <c r="V93" s="31" t="str">
         <f aca="false">IF(AND(K93&lt;&gt;"",K93&lt;&gt;"+3v3",K93&lt;&gt;"GND",NOT(ISNA(P93)),NOT(ISNA(N93))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S93/$V$8,"0.000")," [get_ports {",K93,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S93/$W$8,"0.000")," [get_ports {",K93,"}]",CHAR(10)),"")</f>
@@ -9744,7 +9602,7 @@
       </c>
       <c r="AE93" s="0" t="str">
         <f aca="false">H93</f>
-        <v>tm_n0</v>
+        <v>tm_n1</v>
       </c>
       <c r="AG93" s="8" t="str">
         <f aca="false">IF(OR(LEFT(K93,3)="LED",LEFT(K93,16)="SBUS_DATA_OE_LED"),CONCATENATE("(",CHAR(34),"user_led",CHAR(34),", 0, Pins(",CHAR(34),D93,CHAR(34),"),  IOStandard(",CHAR(34),"lvcmos33",CHAR(34),")), ",CHAR(35),K93),"")</f>
@@ -9778,7 +9636,7 @@
       </c>
       <c r="K94" s="3" t="str">
         <f aca="false">IF(NOT(ISNA($H94)),$H94,"")</f>
-        <v>SD_D3</v>
+        <v>SD_D0</v>
       </c>
       <c r="M94" s="0" t="n">
         <f aca="false">VLOOKUP(A94,'2.13 ping -&gt; trace length'!$A$1:$B$103,2,0)</f>
@@ -9802,9 +9660,8 @@
       </c>
       <c r="U94" s="30" t="str">
         <f aca="false">IF(AND(K94&lt;&gt;"",K94&lt;&gt;"+3v3",K94&lt;&gt;"GND"),CONCATENATE("set_property PACKAGE_PIN ",D94," [get_ports {",K94,"}]",CHAR(10),"set_property IOSTANDARD LVTTL [get_ports {",K94,"}]",CHAR(10)),"")</f>
-        <v>set_property PACKAGE_PIN U1 [get_ports {SD_D3}]
-set_property IOSTANDARD LVTTL [get_ports {SD_D3}]
-</v>
+        <v>set_property PACKAGE_PIN U1 [get_ports {SD_D0}]
+set_property IOSTANDARD LVTTL [get_ports {SD_D0}]</v>
       </c>
       <c r="V94" s="31" t="str">
         <f aca="false">IF(AND(K94&lt;&gt;"",K94&lt;&gt;"+3v3",K94&lt;&gt;"GND",NOT(ISNA(P94)),NOT(ISNA(N94))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S94/$V$8,"0.000")," [get_ports {",K94,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S94/$W$8,"0.000")," [get_ports {",K94,"}]",CHAR(10)),"")</f>
@@ -9831,7 +9688,7 @@
       </c>
       <c r="AE94" s="0" t="str">
         <f aca="false">H94</f>
-        <v>SD_D3</v>
+        <v>SD_D0</v>
       </c>
       <c r="AG94" s="8" t="str">
         <f aca="false">IF(OR(LEFT(K94,3)="LED",LEFT(K94,16)="SBUS_DATA_OE_LED"),CONCATENATE("(",CHAR(34),"user_led",CHAR(34),", 0, Pins(",CHAR(34),D94,CHAR(34),"),  IOStandard(",CHAR(34),"lvcmos33",CHAR(34),")), ",CHAR(35),K94),"")</f>
@@ -9865,7 +9722,7 @@
       </c>
       <c r="K95" s="3" t="str">
         <f aca="false">IF(NOT(ISNA($H95)),$H95,"")</f>
-        <v>tm_n1</v>
+        <v>tm_n0</v>
       </c>
       <c r="M95" s="0" t="n">
         <f aca="false">VLOOKUP(A95,'2.13 ping -&gt; trace length'!$A$1:$B$103,2,0)</f>
@@ -9889,9 +9746,8 @@
       </c>
       <c r="U95" s="30" t="str">
         <f aca="false">IF(AND(K95&lt;&gt;"",K95&lt;&gt;"+3v3",K95&lt;&gt;"GND"),CONCATENATE("set_property PACKAGE_PIN ",D95," [get_ports {",K95,"}]",CHAR(10),"set_property IOSTANDARD LVTTL [get_ports {",K95,"}]",CHAR(10)),"")</f>
-        <v>set_property PACKAGE_PIN U2 [get_ports {tm_n1}]
-set_property IOSTANDARD LVTTL [get_ports {tm_n1}]
-</v>
+        <v>set_property PACKAGE_PIN U2 [get_ports {tm_n0}]
+set_property IOSTANDARD LVTTL [get_ports {tm_n0}]</v>
       </c>
       <c r="V95" s="31" t="str">
         <f aca="false">IF(AND(K95&lt;&gt;"",K95&lt;&gt;"+3v3",K95&lt;&gt;"GND",NOT(ISNA(P95)),NOT(ISNA(N95))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S95/$V$8,"0.000")," [get_ports {",K95,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S95/$W$8,"0.000")," [get_ports {",K95,"}]",CHAR(10)),"")</f>
@@ -9918,7 +9774,7 @@
       </c>
       <c r="AE95" s="0" t="str">
         <f aca="false">H95</f>
-        <v>tm_n1</v>
+        <v>tm_n0</v>
       </c>
       <c r="AG95" s="8" t="str">
         <f aca="false">IF(OR(LEFT(K95,3)="LED",LEFT(K95,16)="SBUS_DATA_OE_LED"),CONCATENATE("(",CHAR(34),"user_led",CHAR(34),", 0, Pins(",CHAR(34),D95,CHAR(34),"),  IOStandard(",CHAR(34),"lvcmos33",CHAR(34),")), ",CHAR(35),K95),"")</f>
@@ -9954,7 +9810,7 @@
       </c>
       <c r="K96" s="3" t="str">
         <f aca="false">IF(NOT(ISNA($H96)),$H96,"")</f>
-        <v>SD_D2</v>
+        <v>SD_D1</v>
       </c>
       <c r="M96" s="0" t="n">
         <f aca="false">VLOOKUP(A96,'2.13 ping -&gt; trace length'!$A$1:$B$103,2,0)</f>
@@ -9978,9 +9834,8 @@
       </c>
       <c r="U96" s="30" t="str">
         <f aca="false">IF(AND(K96&lt;&gt;"",K96&lt;&gt;"+3v3",K96&lt;&gt;"GND"),CONCATENATE("set_property PACKAGE_PIN ",D96," [get_ports {",K96,"}]",CHAR(10),"set_property IOSTANDARD LVTTL [get_ports {",K96,"}]",CHAR(10)),"")</f>
-        <v>set_property PACKAGE_PIN T3 [get_ports {SD_D2}]
-set_property IOSTANDARD LVTTL [get_ports {SD_D2}]
-</v>
+        <v>set_property PACKAGE_PIN T3 [get_ports {SD_D1}]
+set_property IOSTANDARD LVTTL [get_ports {SD_D1}]</v>
       </c>
       <c r="V96" s="31" t="str">
         <f aca="false">IF(AND(K96&lt;&gt;"",K96&lt;&gt;"+3v3",K96&lt;&gt;"GND",NOT(ISNA(P96)),NOT(ISNA(N96))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S96/$V$8,"0.000")," [get_ports {",K96,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S96/$W$8,"0.000")," [get_ports {",K96,"}]",CHAR(10)),"")</f>
@@ -10007,7 +9862,7 @@
       </c>
       <c r="AE96" s="0" t="str">
         <f aca="false">H96</f>
-        <v>SD_D2</v>
+        <v>SD_D1</v>
       </c>
       <c r="AG96" s="8" t="str">
         <f aca="false">IF(OR(LEFT(K96,3)="LED",LEFT(K96,16)="SBUS_DATA_OE_LED"),CONCATENATE("(",CHAR(34),"user_led",CHAR(34),", 0, Pins(",CHAR(34),D96,CHAR(34),"),  IOStandard(",CHAR(34),"lvcmos33",CHAR(34),")), ",CHAR(35),K96),"")</f>
@@ -10068,20 +9923,17 @@
       <c r="U97" s="30" t="str">
         <f aca="false">IF(AND(K97&lt;&gt;"",K97&lt;&gt;"+3v3",K97&lt;&gt;"GND"),CONCATENATE("set_property PACKAGE_PIN ",D97," [get_ports {",K97,"}]",CHAR(10),"set_property IOSTANDARD LVTTL [get_ports {",K97,"}]",CHAR(10)),"")</f>
         <v>set_property PACKAGE_PIN K6 [get_ports {tm_n2}]
-set_property IOSTANDARD LVTTL [get_ports {tm_n2}]
-</v>
+set_property IOSTANDARD LVTTL [get_ports {tm_n2}]</v>
       </c>
       <c r="V97" s="31" t="str">
         <f aca="false">IF(AND(K97&lt;&gt;"",K97&lt;&gt;"+3v3",K97&lt;&gt;"GND",NOT(ISNA(P97)),NOT(ISNA(N97))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S97/$V$8,"0.000")," [get_ports {",K97,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S97/$W$8,"0.000")," [get_ports {",K97,"}]",CHAR(10)),"")</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.704 [get_ports {tm_n2}]
-set_input_delay -clock clk_3v3_n -max 52.855 [get_ports {tm_n2}]
-</v>
+set_input_delay -clock clk_3v3_n -max 52.855 [get_ports {tm_n2}]</v>
       </c>
       <c r="W97" s="31" t="str">
         <f aca="false">IF(AND(K97&lt;&gt;"",K97&lt;&gt;"+3v3",K97&lt;&gt;"GND",NOT(ISNA(P97)),NOT(ISNA(N97))),CONCATENATE("set_output_delay -clock clk_3v3_n -min ",TEXT(-$W$6+P97/$V$8+$P$136/$V$8,"0.000")," [get_ports {",K97,"}]",CHAR(10),"set_output_delay -clock clk_3v3_n -max ",TEXT(0.25+0.25+$W$5+P97/$W$8+$P$136/$W$8,"0.000")," [get_ports {",K97,"}]",CHAR(10)),"")</f>
         <v>set_output_delay -clock clk_3v3_n -min -5.855 [get_ports {tm_n2}]
-set_output_delay -clock clk_3v3_n -max 54.026 [get_ports {tm_n2}]
-</v>
+set_output_delay -clock clk_3v3_n -max 54.026 [get_ports {tm_n2}]</v>
       </c>
       <c r="Y97" s="7" t="str">
         <f aca="false">CONCATENATE(IF(OR(T97="IO",T97="I"),V97,""),IF(OR(T97="IO",T97="O"),W97,""))</f>
@@ -10144,8 +9996,7 @@
       <c r="U98" s="30" t="str">
         <f aca="false">IF(AND(K98&lt;&gt;"",K98&lt;&gt;"+3v3",K98&lt;&gt;"GND"),CONCATENATE("set_property PACKAGE_PIN ",D98," [get_ports {",K98,"}]",CHAR(10),"set_property IOSTANDARD LVTTL [get_ports {",K98,"}]",CHAR(10)),"")</f>
         <v>set_property PACKAGE_PIN R3 [get_ports {reset_n}]
-set_property IOSTANDARD LVTTL [get_ports {reset_n}]
-</v>
+set_property IOSTANDARD LVTTL [get_ports {reset_n}]</v>
       </c>
       <c r="V98" s="31" t="str">
         <f aca="false">IF(AND(K98&lt;&gt;"",K98&lt;&gt;"+3v3",K98&lt;&gt;"GND",NOT(ISNA(P98)),NOT(ISNA(N98))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S98/$V$8,"0.000")," [get_ports {",K98,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S98/$W$8,"0.000")," [get_ports {",K98,"}]",CHAR(10)),"")</f>
@@ -10605,8 +10456,7 @@
       <c r="U105" s="30" t="str">
         <f aca="false">IF(AND(K105&lt;&gt;"",K105&lt;&gt;"+3v3",K105&lt;&gt;"GND"),CONCATENATE("set_property PACKAGE_PIN ",D105," [get_ports {",K105,"}]",CHAR(10),"set_property IOSTANDARD LVTTL [get_ports {",K105,"}]",CHAR(10)),"")</f>
         <v>set_property PACKAGE_PIN N6 [get_ports {HDMI_HPD}]
-set_property IOSTANDARD LVTTL [get_ports {HDMI_HPD}]
-</v>
+set_property IOSTANDARD LVTTL [get_ports {HDMI_HPD}]</v>
       </c>
       <c r="V105" s="31" t="str">
         <f aca="false">IF(AND(K105&lt;&gt;"",K105&lt;&gt;"+3v3",K105&lt;&gt;"GND",NOT(ISNA(P105)),NOT(ISNA(N105))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S105/$V$8,"0.000")," [get_ports {",K105,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S105/$W$8,"0.000")," [get_ports {",K105,"}]",CHAR(10)),"")</f>
@@ -10695,20 +10545,17 @@
       <c r="U106" s="30" t="str">
         <f aca="false">IF(AND(K106&lt;&gt;"",K106&lt;&gt;"+3v3",K106&lt;&gt;"GND"),CONCATENATE("set_property PACKAGE_PIN ",D106," [get_ports {",K106,"}]",CHAR(10),"set_property IOSTANDARD LVTTL [get_ports {",K106,"}]",CHAR(10)),"")</f>
         <v>set_property PACKAGE_PIN P5 [get_ports {PMOD-15}]
-set_property IOSTANDARD LVTTL [get_ports {PMOD-15}]
-</v>
+set_property IOSTANDARD LVTTL [get_ports {PMOD-15}]</v>
       </c>
       <c r="V106" s="31" t="str">
         <f aca="false">IF(AND(K106&lt;&gt;"",K106&lt;&gt;"+3v3",K106&lt;&gt;"GND",NOT(ISNA(P106)),NOT(ISNA(N106))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S106/$V$8,"0.000")," [get_ports {",K106,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S106/$W$8,"0.000")," [get_ports {",K106,"}]",CHAR(10)),"")</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.460 [get_ports {PMOD-15}]
-set_input_delay -clock clk_3v3_n -max 52.530 [get_ports {PMOD-15}]
-</v>
+set_input_delay -clock clk_3v3_n -max 52.530 [get_ports {PMOD-15}]</v>
       </c>
       <c r="W106" s="31" t="str">
         <f aca="false">IF(AND(K106&lt;&gt;"",K106&lt;&gt;"+3v3",K106&lt;&gt;"GND",NOT(ISNA(P106)),NOT(ISNA(N106))),CONCATENATE("set_output_delay -clock clk_3v3_n -min ",TEXT(-$W$6+P106/$V$8+$P$136/$V$8,"0.000")," [get_ports {",K106,"}]",CHAR(10),"set_output_delay -clock clk_3v3_n -max ",TEXT(0.25+0.25+$W$5+P106/$W$8+$P$136/$W$8,"0.000")," [get_ports {",K106,"}]",CHAR(10)),"")</f>
         <v>set_output_delay -clock clk_3v3_n -min -6.099 [get_ports {PMOD-15}]
-set_output_delay -clock clk_3v3_n -max 53.702 [get_ports {PMOD-15}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.702 [get_ports {PMOD-15}]</v>
       </c>
       <c r="Y106" s="7" t="str">
         <f aca="false">CONCATENATE(IF(OR(T106="IO",T106="I"),V106,""),IF(OR(T106="IO",T106="O"),W106,""))</f>
@@ -10787,8 +10634,7 @@
       <c r="U107" s="30" t="str">
         <f aca="false">IF(AND(K107&lt;&gt;"",K107&lt;&gt;"+3v3",K107&lt;&gt;"GND"),CONCATENATE("set_property PACKAGE_PIN ",D107," [get_ports {",K107,"}]",CHAR(10),"set_property IOSTANDARD LVTTL [get_ports {",K107,"}]",CHAR(10)),"")</f>
         <v>set_property PACKAGE_PIN M6 [get_ports {HDMI_SDA}]
-set_property IOSTANDARD LVTTL [get_ports {HDMI_SDA}]
-</v>
+set_property IOSTANDARD LVTTL [get_ports {HDMI_SDA}]</v>
       </c>
       <c r="V107" s="31" t="str">
         <f aca="false">IF(AND(K107&lt;&gt;"",K107&lt;&gt;"+3v3",K107&lt;&gt;"GND",NOT(ISNA(P107)),NOT(ISNA(N107))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S107/$V$8,"0.000")," [get_ports {",K107,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S107/$W$8,"0.000")," [get_ports {",K107,"}]",CHAR(10)),"")</f>
@@ -10877,20 +10723,17 @@
       <c r="U108" s="30" t="str">
         <f aca="false">IF(AND(K108&lt;&gt;"",K108&lt;&gt;"+3v3",K108&lt;&gt;"GND"),CONCATENATE("set_property PACKAGE_PIN ",D108," [get_ports {",K108,"}]",CHAR(10),"set_property IOSTANDARD LVTTL [get_ports {",K108,"}]",CHAR(10)),"")</f>
         <v>set_property PACKAGE_PIN N5 [get_ports {PMOD-16}]
-set_property IOSTANDARD LVTTL [get_ports {PMOD-16}]
-</v>
+set_property IOSTANDARD LVTTL [get_ports {PMOD-16}]</v>
       </c>
       <c r="V108" s="31" t="str">
         <f aca="false">IF(AND(K108&lt;&gt;"",K108&lt;&gt;"+3v3",K108&lt;&gt;"GND",NOT(ISNA(P108)),NOT(ISNA(N108))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S108/$V$8,"0.000")," [get_ports {",K108,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S108/$W$8,"0.000")," [get_ports {",K108,"}]",CHAR(10)),"")</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.460 [get_ports {PMOD-16}]
-set_input_delay -clock clk_3v3_n -max 52.530 [get_ports {PMOD-16}]
-</v>
+set_input_delay -clock clk_3v3_n -max 52.530 [get_ports {PMOD-16}]</v>
       </c>
       <c r="W108" s="31" t="str">
         <f aca="false">IF(AND(K108&lt;&gt;"",K108&lt;&gt;"+3v3",K108&lt;&gt;"GND",NOT(ISNA(P108)),NOT(ISNA(N108))),CONCATENATE("set_output_delay -clock clk_3v3_n -min ",TEXT(-$W$6+P108/$V$8+$P$136/$V$8,"0.000")," [get_ports {",K108,"}]",CHAR(10),"set_output_delay -clock clk_3v3_n -max ",TEXT(0.25+0.25+$W$5+P108/$W$8+$P$136/$W$8,"0.000")," [get_ports {",K108,"}]",CHAR(10)),"")</f>
         <v>set_output_delay -clock clk_3v3_n -min -6.099 [get_ports {PMOD-16}]
-set_output_delay -clock clk_3v3_n -max 53.702 [get_ports {PMOD-16}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.702 [get_ports {PMOD-16}]</v>
       </c>
       <c r="Y108" s="7" t="str">
         <f aca="false">CONCATENATE(IF(OR(T108="IO",T108="I"),V108,""),IF(OR(T108="IO",T108="O"),W108,""))</f>
@@ -10969,8 +10812,7 @@
       <c r="U109" s="30" t="str">
         <f aca="false">IF(AND(K109&lt;&gt;"",K109&lt;&gt;"+3v3",K109&lt;&gt;"GND"),CONCATENATE("set_property PACKAGE_PIN ",D109," [get_ports {",K109,"}]",CHAR(10),"set_property IOSTANDARD LVTTL [get_ports {",K109,"}]",CHAR(10)),"")</f>
         <v>set_property PACKAGE_PIN L6 [get_ports {HDMI_SCL}]
-set_property IOSTANDARD LVTTL [get_ports {HDMI_SCL}]
-</v>
+set_property IOSTANDARD LVTTL [get_ports {HDMI_SCL}]</v>
       </c>
       <c r="V109" s="31" t="str">
         <f aca="false">IF(AND(K109&lt;&gt;"",K109&lt;&gt;"+3v3",K109&lt;&gt;"GND",NOT(ISNA(P109)),NOT(ISNA(N109))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S109/$V$8,"0.000")," [get_ports {",K109,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S109/$W$8,"0.000")," [get_ports {",K109,"}]",CHAR(10)),"")</f>
@@ -11059,20 +10901,17 @@
       <c r="U110" s="30" t="str">
         <f aca="false">IF(AND(K110&lt;&gt;"",K110&lt;&gt;"+3v3",K110&lt;&gt;"GND"),CONCATENATE("set_property PACKAGE_PIN ",D110," [get_ports {",K110,"}]",CHAR(10),"set_property IOSTANDARD LVTTL [get_ports {",K110,"}]",CHAR(10)),"")</f>
         <v>set_property PACKAGE_PIN P4 [get_ports {PMOD-13}]
-set_property IOSTANDARD LVTTL [get_ports {PMOD-13}]
-</v>
+set_property IOSTANDARD LVTTL [get_ports {PMOD-13}]</v>
       </c>
       <c r="V110" s="31" t="str">
         <f aca="false">IF(AND(K110&lt;&gt;"",K110&lt;&gt;"+3v3",K110&lt;&gt;"GND",NOT(ISNA(P110)),NOT(ISNA(N110))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S110/$V$8,"0.000")," [get_ports {",K110,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S110/$W$8,"0.000")," [get_ports {",K110,"}]",CHAR(10)),"")</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.460 [get_ports {PMOD-13}]
-set_input_delay -clock clk_3v3_n -max 52.530 [get_ports {PMOD-13}]
-</v>
+set_input_delay -clock clk_3v3_n -max 52.530 [get_ports {PMOD-13}]</v>
       </c>
       <c r="W110" s="31" t="str">
         <f aca="false">IF(AND(K110&lt;&gt;"",K110&lt;&gt;"+3v3",K110&lt;&gt;"GND",NOT(ISNA(P110)),NOT(ISNA(N110))),CONCATENATE("set_output_delay -clock clk_3v3_n -min ",TEXT(-$W$6+P110/$V$8+$P$136/$V$8,"0.000")," [get_ports {",K110,"}]",CHAR(10),"set_output_delay -clock clk_3v3_n -max ",TEXT(0.25+0.25+$W$5+P110/$W$8+$P$136/$W$8,"0.000")," [get_ports {",K110,"}]",CHAR(10)),"")</f>
         <v>set_output_delay -clock clk_3v3_n -min -6.099 [get_ports {PMOD-13}]
-set_output_delay -clock clk_3v3_n -max 53.702 [get_ports {PMOD-13}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.702 [get_ports {PMOD-13}]</v>
       </c>
       <c r="Y110" s="7" t="str">
         <f aca="false">CONCATENATE(IF(OR(T110="IO",T110="I"),V110,""),IF(OR(T110="IO",T110="O"),W110,""))</f>
@@ -11153,8 +10992,7 @@
       <c r="U111" s="30" t="str">
         <f aca="false">IF(AND(K111&lt;&gt;"",K111&lt;&gt;"+3v3",K111&lt;&gt;"GND"),CONCATENATE("set_property PACKAGE_PIN ",D111," [get_ports {",K111,"}]",CHAR(10),"set_property IOSTANDARD LVTTL [get_ports {",K111,"}]",CHAR(10)),"")</f>
         <v>set_property PACKAGE_PIN L5 [get_ports {HDMI_CEC}]
-set_property IOSTANDARD LVTTL [get_ports {HDMI_CEC}]
-</v>
+set_property IOSTANDARD LVTTL [get_ports {HDMI_CEC}]</v>
       </c>
       <c r="V111" s="31" t="str">
         <f aca="false">IF(AND(K111&lt;&gt;"",K111&lt;&gt;"+3v3",K111&lt;&gt;"GND",NOT(ISNA(P111)),NOT(ISNA(N111))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S111/$V$8,"0.000")," [get_ports {",K111,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S111/$W$8,"0.000")," [get_ports {",K111,"}]",CHAR(10)),"")</f>
@@ -11243,20 +11081,17 @@
       <c r="U112" s="30" t="str">
         <f aca="false">IF(AND(K112&lt;&gt;"",K112&lt;&gt;"+3v3",K112&lt;&gt;"GND"),CONCATENATE("set_property PACKAGE_PIN ",D112," [get_ports {",K112,"}]",CHAR(10),"set_property IOSTANDARD LVTTL [get_ports {",K112,"}]",CHAR(10)),"")</f>
         <v>set_property PACKAGE_PIN P3 [get_ports {PMOD-14}]
-set_property IOSTANDARD LVTTL [get_ports {PMOD-14}]
-</v>
+set_property IOSTANDARD LVTTL [get_ports {PMOD-14}]</v>
       </c>
       <c r="V112" s="31" t="str">
         <f aca="false">IF(AND(K112&lt;&gt;"",K112&lt;&gt;"+3v3",K112&lt;&gt;"GND",NOT(ISNA(P112)),NOT(ISNA(N112))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S112/$V$8,"0.000")," [get_ports {",K112,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S112/$W$8,"0.000")," [get_ports {",K112,"}]",CHAR(10)),"")</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.460 [get_ports {PMOD-14}]
-set_input_delay -clock clk_3v3_n -max 52.530 [get_ports {PMOD-14}]
-</v>
+set_input_delay -clock clk_3v3_n -max 52.530 [get_ports {PMOD-14}]</v>
       </c>
       <c r="W112" s="31" t="str">
         <f aca="false">IF(AND(K112&lt;&gt;"",K112&lt;&gt;"+3v3",K112&lt;&gt;"GND",NOT(ISNA(P112)),NOT(ISNA(N112))),CONCATENATE("set_output_delay -clock clk_3v3_n -min ",TEXT(-$W$6+P112/$V$8+$P$136/$V$8,"0.000")," [get_ports {",K112,"}]",CHAR(10),"set_output_delay -clock clk_3v3_n -max ",TEXT(0.25+0.25+$W$5+P112/$W$8+$P$136/$W$8,"0.000")," [get_ports {",K112,"}]",CHAR(10)),"")</f>
         <v>set_output_delay -clock clk_3v3_n -min -6.099 [get_ports {PMOD-14}]
-set_output_delay -clock clk_3v3_n -max 53.702 [get_ports {PMOD-14}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.702 [get_ports {PMOD-14}]</v>
       </c>
       <c r="Y112" s="7" t="str">
         <f aca="false">CONCATENATE(IF(OR(T112="IO",T112="I"),V112,""),IF(OR(T112="IO",T112="O"),W112,""))</f>
@@ -11335,20 +11170,17 @@
       <c r="U113" s="30" t="str">
         <f aca="false">IF(AND(K113&lt;&gt;"",K113&lt;&gt;"+3v3",K113&lt;&gt;"GND"),CONCATENATE("set_property PACKAGE_PIN ",D113," [get_ports {",K113,"}]",CHAR(10),"set_property IOSTANDARD LVTTL [get_ports {",K113,"}]",CHAR(10)),"")</f>
         <v>set_property PACKAGE_PIN N4 [get_ports {HDMI_CLK-}]
-set_property IOSTANDARD LVTTL [get_ports {HDMI_CLK-}]
-</v>
+set_property IOSTANDARD LVTTL [get_ports {HDMI_CLK-}]</v>
       </c>
       <c r="V113" s="31" t="str">
         <f aca="false">IF(AND(K113&lt;&gt;"",K113&lt;&gt;"+3v3",K113&lt;&gt;"GND",NOT(ISNA(P113)),NOT(ISNA(N113))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S113/$V$8,"0.000")," [get_ports {",K113,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S113/$W$8,"0.000")," [get_ports {",K113,"}]",CHAR(10)),"")</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.429 [get_ports {HDMI_CLK-}]
-set_input_delay -clock clk_3v3_n -max 52.488 [get_ports {HDMI_CLK-}]
-</v>
+set_input_delay -clock clk_3v3_n -max 52.488 [get_ports {HDMI_CLK-}]</v>
       </c>
       <c r="W113" s="31" t="str">
         <f aca="false">IF(AND(K113&lt;&gt;"",K113&lt;&gt;"+3v3",K113&lt;&gt;"GND",NOT(ISNA(P113)),NOT(ISNA(N113))),CONCATENATE("set_output_delay -clock clk_3v3_n -min ",TEXT(-$W$6+P113/$V$8+$P$136/$V$8,"0.000")," [get_ports {",K113,"}]",CHAR(10),"set_output_delay -clock clk_3v3_n -max ",TEXT(0.25+0.25+$W$5+P113/$W$8+$P$136/$W$8,"0.000")," [get_ports {",K113,"}]",CHAR(10)),"")</f>
         <v>set_output_delay -clock clk_3v3_n -min -6.130 [get_ports {HDMI_CLK-}]
-set_output_delay -clock clk_3v3_n -max 53.660 [get_ports {HDMI_CLK-}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.660 [get_ports {HDMI_CLK-}]</v>
       </c>
       <c r="Y113" s="7" t="str">
         <f aca="false">CONCATENATE(IF(OR(T113="IO",T113="I"),V113,""),IF(OR(T113="IO",T113="O"),W113,""))</f>
@@ -11427,20 +11259,17 @@
       <c r="U114" s="30" t="str">
         <f aca="false">IF(AND(K114&lt;&gt;"",K114&lt;&gt;"+3v3",K114&lt;&gt;"GND"),CONCATENATE("set_property PACKAGE_PIN ",D114," [get_ports {",K114,"}]",CHAR(10),"set_property IOSTANDARD LVTTL [get_ports {",K114,"}]",CHAR(10)),"")</f>
         <v>set_property PACKAGE_PIN T1 [get_ports {PMOD-11}]
-set_property IOSTANDARD LVTTL [get_ports {PMOD-11}]
-</v>
+set_property IOSTANDARD LVTTL [get_ports {PMOD-11}]</v>
       </c>
       <c r="V114" s="31" t="str">
         <f aca="false">IF(AND(K114&lt;&gt;"",K114&lt;&gt;"+3v3",K114&lt;&gt;"GND",NOT(ISNA(P114)),NOT(ISNA(N114))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S114/$V$8,"0.000")," [get_ports {",K114,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S114/$W$8,"0.000")," [get_ports {",K114,"}]",CHAR(10)),"")</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.460 [get_ports {PMOD-11}]
-set_input_delay -clock clk_3v3_n -max 52.530 [get_ports {PMOD-11}]
-</v>
+set_input_delay -clock clk_3v3_n -max 52.530 [get_ports {PMOD-11}]</v>
       </c>
       <c r="W114" s="31" t="str">
         <f aca="false">IF(AND(K114&lt;&gt;"",K114&lt;&gt;"+3v3",K114&lt;&gt;"GND",NOT(ISNA(P114)),NOT(ISNA(N114))),CONCATENATE("set_output_delay -clock clk_3v3_n -min ",TEXT(-$W$6+P114/$V$8+$P$136/$V$8,"0.000")," [get_ports {",K114,"}]",CHAR(10),"set_output_delay -clock clk_3v3_n -max ",TEXT(0.25+0.25+$W$5+P114/$W$8+$P$136/$W$8,"0.000")," [get_ports {",K114,"}]",CHAR(10)),"")</f>
         <v>set_output_delay -clock clk_3v3_n -min -6.099 [get_ports {PMOD-11}]
-set_output_delay -clock clk_3v3_n -max 53.702 [get_ports {PMOD-11}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.702 [get_ports {PMOD-11}]</v>
       </c>
       <c r="Y114" s="7" t="str">
         <f aca="false">CONCATENATE(IF(OR(T114="IO",T114="I"),V114,""),IF(OR(T114="IO",T114="O"),W114,""))</f>
@@ -11519,20 +11348,17 @@
       <c r="U115" s="30" t="str">
         <f aca="false">IF(AND(K115&lt;&gt;"",K115&lt;&gt;"+3v3",K115&lt;&gt;"GND"),CONCATENATE("set_property PACKAGE_PIN ",D115," [get_ports {",K115,"}]",CHAR(10),"set_property IOSTANDARD LVTTL [get_ports {",K115,"}]",CHAR(10)),"")</f>
         <v>set_property PACKAGE_PIN M4 [get_ports {HDMI_CLK+}]
-set_property IOSTANDARD LVTTL [get_ports {HDMI_CLK+}]
-</v>
+set_property IOSTANDARD LVTTL [get_ports {HDMI_CLK+}]</v>
       </c>
       <c r="V115" s="31" t="str">
         <f aca="false">IF(AND(K115&lt;&gt;"",K115&lt;&gt;"+3v3",K115&lt;&gt;"GND",NOT(ISNA(P115)),NOT(ISNA(N115))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S115/$V$8,"0.000")," [get_ports {",K115,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S115/$W$8,"0.000")," [get_ports {",K115,"}]",CHAR(10)),"")</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.429 [get_ports {HDMI_CLK+}]
-set_input_delay -clock clk_3v3_n -max 52.488 [get_ports {HDMI_CLK+}]
-</v>
+set_input_delay -clock clk_3v3_n -max 52.488 [get_ports {HDMI_CLK+}]</v>
       </c>
       <c r="W115" s="31" t="str">
         <f aca="false">IF(AND(K115&lt;&gt;"",K115&lt;&gt;"+3v3",K115&lt;&gt;"GND",NOT(ISNA(P115)),NOT(ISNA(N115))),CONCATENATE("set_output_delay -clock clk_3v3_n -min ",TEXT(-$W$6+P115/$V$8+$P$136/$V$8,"0.000")," [get_ports {",K115,"}]",CHAR(10),"set_output_delay -clock clk_3v3_n -max ",TEXT(0.25+0.25+$W$5+P115/$W$8+$P$136/$W$8,"0.000")," [get_ports {",K115,"}]",CHAR(10)),"")</f>
         <v>set_output_delay -clock clk_3v3_n -min -6.130 [get_ports {HDMI_CLK+}]
-set_output_delay -clock clk_3v3_n -max 53.660 [get_ports {HDMI_CLK+}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.660 [get_ports {HDMI_CLK+}]</v>
       </c>
       <c r="Y115" s="7" t="str">
         <f aca="false">CONCATENATE(IF(OR(T115="IO",T115="I"),V115,""),IF(OR(T115="IO",T115="O"),W115,""))</f>
@@ -11611,20 +11437,17 @@
       <c r="U116" s="30" t="str">
         <f aca="false">IF(AND(K116&lt;&gt;"",K116&lt;&gt;"+3v3",K116&lt;&gt;"GND"),CONCATENATE("set_property PACKAGE_PIN ",D116," [get_ports {",K116,"}]",CHAR(10),"set_property IOSTANDARD LVTTL [get_ports {",K116,"}]",CHAR(10)),"")</f>
         <v>set_property PACKAGE_PIN R1 [get_ports {PMOD-12}]
-set_property IOSTANDARD LVTTL [get_ports {PMOD-12}]
-</v>
+set_property IOSTANDARD LVTTL [get_ports {PMOD-12}]</v>
       </c>
       <c r="V116" s="31" t="str">
         <f aca="false">IF(AND(K116&lt;&gt;"",K116&lt;&gt;"+3v3",K116&lt;&gt;"GND",NOT(ISNA(P116)),NOT(ISNA(N116))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S116/$V$8,"0.000")," [get_ports {",K116,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S116/$W$8,"0.000")," [get_ports {",K116,"}]",CHAR(10)),"")</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.460 [get_ports {PMOD-12}]
-set_input_delay -clock clk_3v3_n -max 52.530 [get_ports {PMOD-12}]
-</v>
+set_input_delay -clock clk_3v3_n -max 52.530 [get_ports {PMOD-12}]</v>
       </c>
       <c r="W116" s="31" t="str">
         <f aca="false">IF(AND(K116&lt;&gt;"",K116&lt;&gt;"+3v3",K116&lt;&gt;"GND",NOT(ISNA(P116)),NOT(ISNA(N116))),CONCATENATE("set_output_delay -clock clk_3v3_n -min ",TEXT(-$W$6+P116/$V$8+$P$136/$V$8,"0.000")," [get_ports {",K116,"}]",CHAR(10),"set_output_delay -clock clk_3v3_n -max ",TEXT(0.25+0.25+$W$5+P116/$W$8+$P$136/$W$8,"0.000")," [get_ports {",K116,"}]",CHAR(10)),"")</f>
         <v>set_output_delay -clock clk_3v3_n -min -6.099 [get_ports {PMOD-12}]
-set_output_delay -clock clk_3v3_n -max 53.702 [get_ports {PMOD-12}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.702 [get_ports {PMOD-12}]</v>
       </c>
       <c r="Y116" s="7" t="str">
         <f aca="false">CONCATENATE(IF(OR(T116="IO",T116="I"),V116,""),IF(OR(T116="IO",T116="O"),W116,""))</f>
@@ -11703,20 +11526,17 @@
       <c r="U117" s="30" t="str">
         <f aca="false">IF(AND(K117&lt;&gt;"",K117&lt;&gt;"+3v3",K117&lt;&gt;"GND"),CONCATENATE("set_property PACKAGE_PIN ",D117," [get_ports {",K117,"}]",CHAR(10),"set_property IOSTANDARD LVTTL [get_ports {",K117,"}]",CHAR(10)),"")</f>
         <v>set_property PACKAGE_PIN M3 [get_ports {HDMI_D0+}]
-set_property IOSTANDARD LVTTL [get_ports {HDMI_D0+}]
-</v>
+set_property IOSTANDARD LVTTL [get_ports {HDMI_D0+}]</v>
       </c>
       <c r="V117" s="31" t="str">
         <f aca="false">IF(AND(K117&lt;&gt;"",K117&lt;&gt;"+3v3",K117&lt;&gt;"GND",NOT(ISNA(P117)),NOT(ISNA(N117))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S117/$V$8,"0.000")," [get_ports {",K117,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S117/$W$8,"0.000")," [get_ports {",K117,"}]",CHAR(10)),"")</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.429 [get_ports {HDMI_D0+}]
-set_input_delay -clock clk_3v3_n -max 52.488 [get_ports {HDMI_D0+}]
-</v>
+set_input_delay -clock clk_3v3_n -max 52.488 [get_ports {HDMI_D0+}]</v>
       </c>
       <c r="W117" s="31" t="str">
         <f aca="false">IF(AND(K117&lt;&gt;"",K117&lt;&gt;"+3v3",K117&lt;&gt;"GND",NOT(ISNA(P117)),NOT(ISNA(N117))),CONCATENATE("set_output_delay -clock clk_3v3_n -min ",TEXT(-$W$6+P117/$V$8+$P$136/$V$8,"0.000")," [get_ports {",K117,"}]",CHAR(10),"set_output_delay -clock clk_3v3_n -max ",TEXT(0.25+0.25+$W$5+P117/$W$8+$P$136/$W$8,"0.000")," [get_ports {",K117,"}]",CHAR(10)),"")</f>
         <v>set_output_delay -clock clk_3v3_n -min -6.130 [get_ports {HDMI_D0+}]
-set_output_delay -clock clk_3v3_n -max 53.660 [get_ports {HDMI_D0+}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.660 [get_ports {HDMI_D0+}]</v>
       </c>
       <c r="Y117" s="7" t="str">
         <f aca="false">CONCATENATE(IF(OR(T117="IO",T117="I"),V117,""),IF(OR(T117="IO",T117="O"),W117,""))</f>
@@ -11795,20 +11615,17 @@
       <c r="U118" s="30" t="str">
         <f aca="false">IF(AND(K118&lt;&gt;"",K118&lt;&gt;"+3v3",K118&lt;&gt;"GND"),CONCATENATE("set_property PACKAGE_PIN ",D118," [get_ports {",K118,"}]",CHAR(10),"set_property IOSTANDARD LVTTL [get_ports {",K118,"}]",CHAR(10)),"")</f>
         <v>set_property PACKAGE_PIN R2 [get_ports {PMOD-9}]
-set_property IOSTANDARD LVTTL [get_ports {PMOD-9}]
-</v>
+set_property IOSTANDARD LVTTL [get_ports {PMOD-9}]</v>
       </c>
       <c r="V118" s="31" t="str">
         <f aca="false">IF(AND(K118&lt;&gt;"",K118&lt;&gt;"+3v3",K118&lt;&gt;"GND",NOT(ISNA(P118)),NOT(ISNA(N118))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S118/$V$8,"0.000")," [get_ports {",K118,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S118/$W$8,"0.000")," [get_ports {",K118,"}]",CHAR(10)),"")</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.460 [get_ports {PMOD-9}]
-set_input_delay -clock clk_3v3_n -max 52.530 [get_ports {PMOD-9}]
-</v>
+set_input_delay -clock clk_3v3_n -max 52.530 [get_ports {PMOD-9}]</v>
       </c>
       <c r="W118" s="31" t="str">
         <f aca="false">IF(AND(K118&lt;&gt;"",K118&lt;&gt;"+3v3",K118&lt;&gt;"GND",NOT(ISNA(P118)),NOT(ISNA(N118))),CONCATENATE("set_output_delay -clock clk_3v3_n -min ",TEXT(-$W$6+P118/$V$8+$P$136/$V$8,"0.000")," [get_ports {",K118,"}]",CHAR(10),"set_output_delay -clock clk_3v3_n -max ",TEXT(0.25+0.25+$W$5+P118/$W$8+$P$136/$W$8,"0.000")," [get_ports {",K118,"}]",CHAR(10)),"")</f>
         <v>set_output_delay -clock clk_3v3_n -min -6.099 [get_ports {PMOD-9}]
-set_output_delay -clock clk_3v3_n -max 53.702 [get_ports {PMOD-9}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.702 [get_ports {PMOD-9}]</v>
       </c>
       <c r="Y118" s="7" t="str">
         <f aca="false">CONCATENATE(IF(OR(T118="IO",T118="I"),V118,""),IF(OR(T118="IO",T118="O"),W118,""))</f>
@@ -11887,20 +11704,17 @@
       <c r="U119" s="30" t="str">
         <f aca="false">IF(AND(K119&lt;&gt;"",K119&lt;&gt;"+3v3",K119&lt;&gt;"GND"),CONCATENATE("set_property PACKAGE_PIN ",D119," [get_ports {",K119,"}]",CHAR(10),"set_property IOSTANDARD LVTTL [get_ports {",K119,"}]",CHAR(10)),"")</f>
         <v>set_property PACKAGE_PIN M2 [get_ports {HDMI_D0-}]
-set_property IOSTANDARD LVTTL [get_ports {HDMI_D0-}]
-</v>
+set_property IOSTANDARD LVTTL [get_ports {HDMI_D0-}]</v>
       </c>
       <c r="V119" s="31" t="str">
         <f aca="false">IF(AND(K119&lt;&gt;"",K119&lt;&gt;"+3v3",K119&lt;&gt;"GND",NOT(ISNA(P119)),NOT(ISNA(N119))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S119/$V$8,"0.000")," [get_ports {",K119,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S119/$W$8,"0.000")," [get_ports {",K119,"}]",CHAR(10)),"")</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.429 [get_ports {HDMI_D0-}]
-set_input_delay -clock clk_3v3_n -max 52.488 [get_ports {HDMI_D0-}]
-</v>
+set_input_delay -clock clk_3v3_n -max 52.488 [get_ports {HDMI_D0-}]</v>
       </c>
       <c r="W119" s="31" t="str">
         <f aca="false">IF(AND(K119&lt;&gt;"",K119&lt;&gt;"+3v3",K119&lt;&gt;"GND",NOT(ISNA(P119)),NOT(ISNA(N119))),CONCATENATE("set_output_delay -clock clk_3v3_n -min ",TEXT(-$W$6+P119/$V$8+$P$136/$V$8,"0.000")," [get_ports {",K119,"}]",CHAR(10),"set_output_delay -clock clk_3v3_n -max ",TEXT(0.25+0.25+$W$5+P119/$W$8+$P$136/$W$8,"0.000")," [get_ports {",K119,"}]",CHAR(10)),"")</f>
         <v>set_output_delay -clock clk_3v3_n -min -6.130 [get_ports {HDMI_D0-}]
-set_output_delay -clock clk_3v3_n -max 53.660 [get_ports {HDMI_D0-}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.660 [get_ports {HDMI_D0-}]</v>
       </c>
       <c r="Y119" s="7" t="str">
         <f aca="false">CONCATENATE(IF(OR(T119="IO",T119="I"),V119,""),IF(OR(T119="IO",T119="O"),W119,""))</f>
@@ -11979,20 +11793,17 @@
       <c r="U120" s="30" t="str">
         <f aca="false">IF(AND(K120&lt;&gt;"",K120&lt;&gt;"+3v3",K120&lt;&gt;"GND"),CONCATENATE("set_property PACKAGE_PIN ",D120," [get_ports {",K120,"}]",CHAR(10),"set_property IOSTANDARD LVTTL [get_ports {",K120,"}]",CHAR(10)),"")</f>
         <v>set_property PACKAGE_PIN P2 [get_ports {PMOD-10}]
-set_property IOSTANDARD LVTTL [get_ports {PMOD-10}]
-</v>
+set_property IOSTANDARD LVTTL [get_ports {PMOD-10}]</v>
       </c>
       <c r="V120" s="31" t="str">
         <f aca="false">IF(AND(K120&lt;&gt;"",K120&lt;&gt;"+3v3",K120&lt;&gt;"GND",NOT(ISNA(P120)),NOT(ISNA(N120))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S120/$V$8,"0.000")," [get_ports {",K120,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S120/$W$8,"0.000")," [get_ports {",K120,"}]",CHAR(10)),"")</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.460 [get_ports {PMOD-10}]
-set_input_delay -clock clk_3v3_n -max 52.530 [get_ports {PMOD-10}]
-</v>
+set_input_delay -clock clk_3v3_n -max 52.530 [get_ports {PMOD-10}]</v>
       </c>
       <c r="W120" s="31" t="str">
         <f aca="false">IF(AND(K120&lt;&gt;"",K120&lt;&gt;"+3v3",K120&lt;&gt;"GND",NOT(ISNA(P120)),NOT(ISNA(N120))),CONCATENATE("set_output_delay -clock clk_3v3_n -min ",TEXT(-$W$6+P120/$V$8+$P$136/$V$8,"0.000")," [get_ports {",K120,"}]",CHAR(10),"set_output_delay -clock clk_3v3_n -max ",TEXT(0.25+0.25+$W$5+P120/$W$8+$P$136/$W$8,"0.000")," [get_ports {",K120,"}]",CHAR(10)),"")</f>
         <v>set_output_delay -clock clk_3v3_n -min -6.099 [get_ports {PMOD-10}]
-set_output_delay -clock clk_3v3_n -max 53.702 [get_ports {PMOD-10}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.702 [get_ports {PMOD-10}]</v>
       </c>
       <c r="Y120" s="7" t="str">
         <f aca="false">CONCATENATE(IF(OR(T120="IO",T120="I"),V120,""),IF(OR(T120="IO",T120="O"),W120,""))</f>
@@ -12071,20 +11882,17 @@
       <c r="U121" s="30" t="str">
         <f aca="false">IF(AND(K121&lt;&gt;"",K121&lt;&gt;"+3v3",K121&lt;&gt;"GND"),CONCATENATE("set_property PACKAGE_PIN ",D121," [get_ports {",K121,"}]",CHAR(10),"set_property IOSTANDARD LVTTL [get_ports {",K121,"}]",CHAR(10)),"")</f>
         <v>set_property PACKAGE_PIN K5 [get_ports {HDMI_D1+}]
-set_property IOSTANDARD LVTTL [get_ports {HDMI_D1+}]
-</v>
+set_property IOSTANDARD LVTTL [get_ports {HDMI_D1+}]</v>
       </c>
       <c r="V121" s="31" t="str">
         <f aca="false">IF(AND(K121&lt;&gt;"",K121&lt;&gt;"+3v3",K121&lt;&gt;"GND",NOT(ISNA(P121)),NOT(ISNA(N121))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S121/$V$8,"0.000")," [get_ports {",K121,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S121/$W$8,"0.000")," [get_ports {",K121,"}]",CHAR(10)),"")</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.429 [get_ports {HDMI_D1+}]
-set_input_delay -clock clk_3v3_n -max 52.488 [get_ports {HDMI_D1+}]
-</v>
+set_input_delay -clock clk_3v3_n -max 52.488 [get_ports {HDMI_D1+}]</v>
       </c>
       <c r="W121" s="31" t="str">
         <f aca="false">IF(AND(K121&lt;&gt;"",K121&lt;&gt;"+3v3",K121&lt;&gt;"GND",NOT(ISNA(P121)),NOT(ISNA(N121))),CONCATENATE("set_output_delay -clock clk_3v3_n -min ",TEXT(-$W$6+P121/$V$8+$P$136/$V$8,"0.000")," [get_ports {",K121,"}]",CHAR(10),"set_output_delay -clock clk_3v3_n -max ",TEXT(0.25+0.25+$W$5+P121/$W$8+$P$136/$W$8,"0.000")," [get_ports {",K121,"}]",CHAR(10)),"")</f>
         <v>set_output_delay -clock clk_3v3_n -min -6.130 [get_ports {HDMI_D1+}]
-set_output_delay -clock clk_3v3_n -max 53.660 [get_ports {HDMI_D1+}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.660 [get_ports {HDMI_D1+}]</v>
       </c>
       <c r="Y121" s="7" t="str">
         <f aca="false">CONCATENATE(IF(OR(T121="IO",T121="I"),V121,""),IF(OR(T121="IO",T121="O"),W121,""))</f>
@@ -12163,20 +11971,17 @@
       <c r="U122" s="30" t="str">
         <f aca="false">IF(AND(K122&lt;&gt;"",K122&lt;&gt;"+3v3",K122&lt;&gt;"GND"),CONCATENATE("set_property PACKAGE_PIN ",D122," [get_ports {",K122,"}]",CHAR(10),"set_property IOSTANDARD LVTTL [get_ports {",K122,"}]",CHAR(10)),"")</f>
         <v>set_property PACKAGE_PIN N2 [get_ports {PMOD-7}]
-set_property IOSTANDARD LVTTL [get_ports {PMOD-7}]
-</v>
+set_property IOSTANDARD LVTTL [get_ports {PMOD-7}]</v>
       </c>
       <c r="V122" s="31" t="str">
         <f aca="false">IF(AND(K122&lt;&gt;"",K122&lt;&gt;"+3v3",K122&lt;&gt;"GND",NOT(ISNA(P122)),NOT(ISNA(N122))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S122/$V$8,"0.000")," [get_ports {",K122,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S122/$W$8,"0.000")," [get_ports {",K122,"}]",CHAR(10)),"")</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.460 [get_ports {PMOD-7}]
-set_input_delay -clock clk_3v3_n -max 52.530 [get_ports {PMOD-7}]
-</v>
+set_input_delay -clock clk_3v3_n -max 52.530 [get_ports {PMOD-7}]</v>
       </c>
       <c r="W122" s="31" t="str">
         <f aca="false">IF(AND(K122&lt;&gt;"",K122&lt;&gt;"+3v3",K122&lt;&gt;"GND",NOT(ISNA(P122)),NOT(ISNA(N122))),CONCATENATE("set_output_delay -clock clk_3v3_n -min ",TEXT(-$W$6+P122/$V$8+$P$136/$V$8,"0.000")," [get_ports {",K122,"}]",CHAR(10),"set_output_delay -clock clk_3v3_n -max ",TEXT(0.25+0.25+$W$5+P122/$W$8+$P$136/$W$8,"0.000")," [get_ports {",K122,"}]",CHAR(10)),"")</f>
         <v>set_output_delay -clock clk_3v3_n -min -6.099 [get_ports {PMOD-7}]
-set_output_delay -clock clk_3v3_n -max 53.702 [get_ports {PMOD-7}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.702 [get_ports {PMOD-7}]</v>
       </c>
       <c r="Y122" s="7" t="str">
         <f aca="false">CONCATENATE(IF(OR(T122="IO",T122="I"),V122,""),IF(OR(T122="IO",T122="O"),W122,""))</f>
@@ -12255,20 +12060,17 @@
       <c r="U123" s="30" t="str">
         <f aca="false">IF(AND(K123&lt;&gt;"",K123&lt;&gt;"+3v3",K123&lt;&gt;"GND"),CONCATENATE("set_property PACKAGE_PIN ",D123," [get_ports {",K123,"}]",CHAR(10),"set_property IOSTANDARD LVTTL [get_ports {",K123,"}]",CHAR(10)),"")</f>
         <v>set_property PACKAGE_PIN L4 [get_ports {HDMI_D1-}]
-set_property IOSTANDARD LVTTL [get_ports {HDMI_D1-}]
-</v>
+set_property IOSTANDARD LVTTL [get_ports {HDMI_D1-}]</v>
       </c>
       <c r="V123" s="31" t="str">
         <f aca="false">IF(AND(K123&lt;&gt;"",K123&lt;&gt;"+3v3",K123&lt;&gt;"GND",NOT(ISNA(P123)),NOT(ISNA(N123))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S123/$V$8,"0.000")," [get_ports {",K123,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S123/$W$8,"0.000")," [get_ports {",K123,"}]",CHAR(10)),"")</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.429 [get_ports {HDMI_D1-}]
-set_input_delay -clock clk_3v3_n -max 52.488 [get_ports {HDMI_D1-}]
-</v>
+set_input_delay -clock clk_3v3_n -max 52.488 [get_ports {HDMI_D1-}]</v>
       </c>
       <c r="W123" s="31" t="str">
         <f aca="false">IF(AND(K123&lt;&gt;"",K123&lt;&gt;"+3v3",K123&lt;&gt;"GND",NOT(ISNA(P123)),NOT(ISNA(N123))),CONCATENATE("set_output_delay -clock clk_3v3_n -min ",TEXT(-$W$6+P123/$V$8+$P$136/$V$8,"0.000")," [get_ports {",K123,"}]",CHAR(10),"set_output_delay -clock clk_3v3_n -max ",TEXT(0.25+0.25+$W$5+P123/$W$8+$P$136/$W$8,"0.000")," [get_ports {",K123,"}]",CHAR(10)),"")</f>
         <v>set_output_delay -clock clk_3v3_n -min -6.130 [get_ports {HDMI_D1-}]
-set_output_delay -clock clk_3v3_n -max 53.660 [get_ports {HDMI_D1-}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.660 [get_ports {HDMI_D1-}]</v>
       </c>
       <c r="Y123" s="7" t="str">
         <f aca="false">CONCATENATE(IF(OR(T123="IO",T123="I"),V123,""),IF(OR(T123="IO",T123="O"),W123,""))</f>
@@ -12347,20 +12149,17 @@
       <c r="U124" s="30" t="str">
         <f aca="false">IF(AND(K124&lt;&gt;"",K124&lt;&gt;"+3v3",K124&lt;&gt;"GND"),CONCATENATE("set_property PACKAGE_PIN ",D124," [get_ports {",K124,"}]",CHAR(10),"set_property IOSTANDARD LVTTL [get_ports {",K124,"}]",CHAR(10)),"")</f>
         <v>set_property PACKAGE_PIN N1 [get_ports {PMOD-8}]
-set_property IOSTANDARD LVTTL [get_ports {PMOD-8}]
-</v>
+set_property IOSTANDARD LVTTL [get_ports {PMOD-8}]</v>
       </c>
       <c r="V124" s="31" t="str">
         <f aca="false">IF(AND(K124&lt;&gt;"",K124&lt;&gt;"+3v3",K124&lt;&gt;"GND",NOT(ISNA(P124)),NOT(ISNA(N124))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S124/$V$8,"0.000")," [get_ports {",K124,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S124/$W$8,"0.000")," [get_ports {",K124,"}]",CHAR(10)),"")</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.460 [get_ports {PMOD-8}]
-set_input_delay -clock clk_3v3_n -max 52.530 [get_ports {PMOD-8}]
-</v>
+set_input_delay -clock clk_3v3_n -max 52.530 [get_ports {PMOD-8}]</v>
       </c>
       <c r="W124" s="31" t="str">
         <f aca="false">IF(AND(K124&lt;&gt;"",K124&lt;&gt;"+3v3",K124&lt;&gt;"GND",NOT(ISNA(P124)),NOT(ISNA(N124))),CONCATENATE("set_output_delay -clock clk_3v3_n -min ",TEXT(-$W$6+P124/$V$8+$P$136/$V$8,"0.000")," [get_ports {",K124,"}]",CHAR(10),"set_output_delay -clock clk_3v3_n -max ",TEXT(0.25+0.25+$W$5+P124/$W$8+$P$136/$W$8,"0.000")," [get_ports {",K124,"}]",CHAR(10)),"")</f>
         <v>set_output_delay -clock clk_3v3_n -min -6.099 [get_ports {PMOD-8}]
-set_output_delay -clock clk_3v3_n -max 53.702 [get_ports {PMOD-8}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.702 [get_ports {PMOD-8}]</v>
       </c>
       <c r="Y124" s="7" t="str">
         <f aca="false">CONCATENATE(IF(OR(T124="IO",T124="I"),V124,""),IF(OR(T124="IO",T124="O"),W124,""))</f>
@@ -12439,20 +12238,17 @@
       <c r="U125" s="30" t="str">
         <f aca="false">IF(AND(K125&lt;&gt;"",K125&lt;&gt;"+3v3",K125&lt;&gt;"GND"),CONCATENATE("set_property PACKAGE_PIN ",D125," [get_ports {",K125,"}]",CHAR(10),"set_property IOSTANDARD LVTTL [get_ports {",K125,"}]",CHAR(10)),"")</f>
         <v>set_property PACKAGE_PIN L3 [get_ports {HDMI_D2-}]
-set_property IOSTANDARD LVTTL [get_ports {HDMI_D2-}]
-</v>
+set_property IOSTANDARD LVTTL [get_ports {HDMI_D2-}]</v>
       </c>
       <c r="V125" s="31" t="str">
         <f aca="false">IF(AND(K125&lt;&gt;"",K125&lt;&gt;"+3v3",K125&lt;&gt;"GND",NOT(ISNA(P125)),NOT(ISNA(N125))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S125/$V$8,"0.000")," [get_ports {",K125,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S125/$W$8,"0.000")," [get_ports {",K125,"}]",CHAR(10)),"")</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.429 [get_ports {HDMI_D2-}]
-set_input_delay -clock clk_3v3_n -max 52.488 [get_ports {HDMI_D2-}]
-</v>
+set_input_delay -clock clk_3v3_n -max 52.488 [get_ports {HDMI_D2-}]</v>
       </c>
       <c r="W125" s="31" t="str">
         <f aca="false">IF(AND(K125&lt;&gt;"",K125&lt;&gt;"+3v3",K125&lt;&gt;"GND",NOT(ISNA(P125)),NOT(ISNA(N125))),CONCATENATE("set_output_delay -clock clk_3v3_n -min ",TEXT(-$W$6+P125/$V$8+$P$136/$V$8,"0.000")," [get_ports {",K125,"}]",CHAR(10),"set_output_delay -clock clk_3v3_n -max ",TEXT(0.25+0.25+$W$5+P125/$W$8+$P$136/$W$8,"0.000")," [get_ports {",K125,"}]",CHAR(10)),"")</f>
         <v>set_output_delay -clock clk_3v3_n -min -6.130 [get_ports {HDMI_D2-}]
-set_output_delay -clock clk_3v3_n -max 53.660 [get_ports {HDMI_D2-}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.660 [get_ports {HDMI_D2-}]</v>
       </c>
       <c r="Y125" s="7" t="str">
         <f aca="false">CONCATENATE(IF(OR(T125="IO",T125="I"),V125,""),IF(OR(T125="IO",T125="O"),W125,""))</f>
@@ -12531,20 +12327,17 @@
       <c r="U126" s="30" t="str">
         <f aca="false">IF(AND(K126&lt;&gt;"",K126&lt;&gt;"+3v3",K126&lt;&gt;"GND"),CONCATENATE("set_property PACKAGE_PIN ",D126," [get_ports {",K126,"}]",CHAR(10),"set_property IOSTANDARD LVTTL [get_ports {",K126,"}]",CHAR(10)),"")</f>
         <v>set_property PACKAGE_PIN M1 [get_ports {PMOD-5}]
-set_property IOSTANDARD LVTTL [get_ports {PMOD-5}]
-</v>
+set_property IOSTANDARD LVTTL [get_ports {PMOD-5}]</v>
       </c>
       <c r="V126" s="31" t="str">
         <f aca="false">IF(AND(K126&lt;&gt;"",K126&lt;&gt;"+3v3",K126&lt;&gt;"GND",NOT(ISNA(P126)),NOT(ISNA(N126))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S126/$V$8,"0.000")," [get_ports {",K126,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S126/$W$8,"0.000")," [get_ports {",K126,"}]",CHAR(10)),"")</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.460 [get_ports {PMOD-5}]
-set_input_delay -clock clk_3v3_n -max 52.530 [get_ports {PMOD-5}]
-</v>
+set_input_delay -clock clk_3v3_n -max 52.530 [get_ports {PMOD-5}]</v>
       </c>
       <c r="W126" s="31" t="str">
         <f aca="false">IF(AND(K126&lt;&gt;"",K126&lt;&gt;"+3v3",K126&lt;&gt;"GND",NOT(ISNA(P126)),NOT(ISNA(N126))),CONCATENATE("set_output_delay -clock clk_3v3_n -min ",TEXT(-$W$6+P126/$V$8+$P$136/$V$8,"0.000")," [get_ports {",K126,"}]",CHAR(10),"set_output_delay -clock clk_3v3_n -max ",TEXT(0.25+0.25+$W$5+P126/$W$8+$P$136/$W$8,"0.000")," [get_ports {",K126,"}]",CHAR(10)),"")</f>
         <v>set_output_delay -clock clk_3v3_n -min -6.099 [get_ports {PMOD-5}]
-set_output_delay -clock clk_3v3_n -max 53.702 [get_ports {PMOD-5}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.702 [get_ports {PMOD-5}]</v>
       </c>
       <c r="Y126" s="7" t="str">
         <f aca="false">CONCATENATE(IF(OR(T126="IO",T126="I"),V126,""),IF(OR(T126="IO",T126="O"),W126,""))</f>
@@ -12623,20 +12416,17 @@
       <c r="U127" s="30" t="str">
         <f aca="false">IF(AND(K127&lt;&gt;"",K127&lt;&gt;"+3v3",K127&lt;&gt;"GND"),CONCATENATE("set_property PACKAGE_PIN ",D127," [get_ports {",K127,"}]",CHAR(10),"set_property IOSTANDARD LVTTL [get_ports {",K127,"}]",CHAR(10)),"")</f>
         <v>set_property PACKAGE_PIN K3 [get_ports {HDMI_D2+}]
-set_property IOSTANDARD LVTTL [get_ports {HDMI_D2+}]
-</v>
+set_property IOSTANDARD LVTTL [get_ports {HDMI_D2+}]</v>
       </c>
       <c r="V127" s="31" t="str">
         <f aca="false">IF(AND(K127&lt;&gt;"",K127&lt;&gt;"+3v3",K127&lt;&gt;"GND",NOT(ISNA(P127)),NOT(ISNA(N127))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S127/$V$8,"0.000")," [get_ports {",K127,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S127/$W$8,"0.000")," [get_ports {",K127,"}]",CHAR(10)),"")</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.429 [get_ports {HDMI_D2+}]
-set_input_delay -clock clk_3v3_n -max 52.488 [get_ports {HDMI_D2+}]
-</v>
+set_input_delay -clock clk_3v3_n -max 52.488 [get_ports {HDMI_D2+}]</v>
       </c>
       <c r="W127" s="31" t="str">
         <f aca="false">IF(AND(K127&lt;&gt;"",K127&lt;&gt;"+3v3",K127&lt;&gt;"GND",NOT(ISNA(P127)),NOT(ISNA(N127))),CONCATENATE("set_output_delay -clock clk_3v3_n -min ",TEXT(-$W$6+P127/$V$8+$P$136/$V$8,"0.000")," [get_ports {",K127,"}]",CHAR(10),"set_output_delay -clock clk_3v3_n -max ",TEXT(0.25+0.25+$W$5+P127/$W$8+$P$136/$W$8,"0.000")," [get_ports {",K127,"}]",CHAR(10)),"")</f>
         <v>set_output_delay -clock clk_3v3_n -min -6.130 [get_ports {HDMI_D2+}]
-set_output_delay -clock clk_3v3_n -max 53.660 [get_ports {HDMI_D2+}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.660 [get_ports {HDMI_D2+}]</v>
       </c>
       <c r="Y127" s="7" t="str">
         <f aca="false">CONCATENATE(IF(OR(T127="IO",T127="I"),V127,""),IF(OR(T127="IO",T127="O"),W127,""))</f>
@@ -12715,20 +12505,17 @@
       <c r="U128" s="30" t="str">
         <f aca="false">IF(AND(K128&lt;&gt;"",K128&lt;&gt;"+3v3",K128&lt;&gt;"GND"),CONCATENATE("set_property PACKAGE_PIN ",D128," [get_ports {",K128,"}]",CHAR(10),"set_property IOSTANDARD LVTTL [get_ports {",K128,"}]",CHAR(10)),"")</f>
         <v>set_property PACKAGE_PIN L1 [get_ports {PMOD-6}]
-set_property IOSTANDARD LVTTL [get_ports {PMOD-6}]
-</v>
+set_property IOSTANDARD LVTTL [get_ports {PMOD-6}]</v>
       </c>
       <c r="V128" s="31" t="str">
         <f aca="false">IF(AND(K128&lt;&gt;"",K128&lt;&gt;"+3v3",K128&lt;&gt;"GND",NOT(ISNA(P128)),NOT(ISNA(N128))),CONCATENATE("set_input_delay -clock clk_3v3_n -min ",TEXT(-0.25+$V$6-S128/$V$8,"0.000")," [get_ports {",K128,"}]",CHAR(10),"set_input_delay -clock clk_3v3_n -max ",TEXT(0.25+(100-$V$5)-S128/$W$8,"0.000")," [get_ports {",K128,"}]",CHAR(10)),"")</f>
         <v>set_input_delay -clock clk_3v3_n -min 2.460 [get_ports {PMOD-6}]
-set_input_delay -clock clk_3v3_n -max 52.530 [get_ports {PMOD-6}]
-</v>
+set_input_delay -clock clk_3v3_n -max 52.530 [get_ports {PMOD-6}]</v>
       </c>
       <c r="W128" s="31" t="str">
         <f aca="false">IF(AND(K128&lt;&gt;"",K128&lt;&gt;"+3v3",K128&lt;&gt;"GND",NOT(ISNA(P128)),NOT(ISNA(N128))),CONCATENATE("set_output_delay -clock clk_3v3_n -min ",TEXT(-$W$6+P128/$V$8+$P$136/$V$8,"0.000")," [get_ports {",K128,"}]",CHAR(10),"set_output_delay -clock clk_3v3_n -max ",TEXT(0.25+0.25+$W$5+P128/$W$8+$P$136/$W$8,"0.000")," [get_ports {",K128,"}]",CHAR(10)),"")</f>
         <v>set_output_delay -clock clk_3v3_n -min -6.099 [get_ports {PMOD-6}]
-set_output_delay -clock clk_3v3_n -max 53.702 [get_ports {PMOD-6}]
-</v>
+set_output_delay -clock clk_3v3_n -max 53.702 [get_ports {PMOD-6}]</v>
       </c>
       <c r="Y128" s="7" t="str">
         <f aca="false">CONCATENATE(IF(OR(T128="IO",T128="I"),V128,""),IF(OR(T128="IO",T128="O"),W128,""))</f>
@@ -15890,7 +15677,7 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>335</v>
+        <v>341</v>
       </c>
       <c r="B43" s="115" t="n">
         <v>28340036.0603</v>
@@ -15905,7 +15692,7 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="B44" s="115" t="n">
         <v>28993590.7628</v>

</xml_diff>